<commit_message>
assesment testcases updated final
</commit_message>
<xml_diff>
--- a/Assessment_Testcases.xlsx
+++ b/Assessment_Testcases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MyLocal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2991741-C77C-4162-A9BA-6797D1A8757D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43F781E2-32A4-4FC5-980D-21789D31477B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8F82FB5E-0F38-4637-B99A-510675DA02B5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="322">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -1110,7 +1110,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1164,34 +1164,19 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1202,11 +1187,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1603,9 +1600,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCDC6287-C9DF-48D0-A699-A65D1ACAEAC9}">
   <dimension ref="A1:L139"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K75" sqref="K75:K79"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H110" sqref="H110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1664,104 +1661,104 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="18" t="s">
-        <v>246</v>
-      </c>
-      <c r="C2" s="20" t="s">
+      <c r="B2" s="20" t="s">
+        <v>246</v>
+      </c>
+      <c r="C2" s="29" t="s">
         <v>142</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="29" t="s">
         <v>192</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="29" t="s">
         <v>248</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="29" t="s">
         <v>310</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="H2" s="29" t="s">
         <v>222</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="29" t="s">
         <v>305</v>
       </c>
-      <c r="J2" s="20" t="s">
+      <c r="J2" s="29" t="s">
         <v>319</v>
       </c>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="19"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
+      <c r="A3" s="28"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
       <c r="F3" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="B4" s="18" t="s">
-        <v>246</v>
-      </c>
-      <c r="C4" s="20" t="s">
+      <c r="B4" s="20" t="s">
+        <v>246</v>
+      </c>
+      <c r="C4" s="29" t="s">
         <v>142</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="29" t="s">
         <v>193</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="29" t="s">
         <v>248</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="G4" s="20" t="s">
+      <c r="G4" s="29" t="s">
         <v>310</v>
       </c>
-      <c r="H4" s="20" t="s">
+      <c r="H4" s="29" t="s">
         <v>223</v>
       </c>
-      <c r="I4" s="20" t="s">
+      <c r="I4" s="29" t="s">
         <v>305</v>
       </c>
-      <c r="J4" s="20" t="s">
+      <c r="J4" s="29" t="s">
         <v>319</v>
       </c>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="29"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="19"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
+      <c r="A5" s="28"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
       <c r="F5" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="29"/>
     </row>
     <row r="6" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
@@ -1782,7 +1779,7 @@
       <c r="F6" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="G6" s="31" t="s">
+      <c r="G6" s="12" t="s">
         <v>311</v>
       </c>
       <c r="H6" s="8" t="s">
@@ -1866,58 +1863,58 @@
       <c r="L8" s="8"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="B9" s="18" t="s">
-        <v>246</v>
-      </c>
-      <c r="C9" s="20" t="s">
+      <c r="B9" s="20" t="s">
+        <v>246</v>
+      </c>
+      <c r="C9" s="29" t="s">
         <v>143</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="29" t="s">
         <v>197</v>
       </c>
-      <c r="E9" s="20" t="s">
+      <c r="E9" s="29" t="s">
         <v>248</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>213</v>
       </c>
-      <c r="G9" s="20" t="s">
+      <c r="G9" s="29" t="s">
         <v>310</v>
       </c>
-      <c r="H9" s="20" t="s">
+      <c r="H9" s="29" t="s">
         <v>244</v>
       </c>
-      <c r="I9" s="20" t="s">
+      <c r="I9" s="29" t="s">
         <v>305</v>
       </c>
-      <c r="J9" s="20" t="s">
+      <c r="J9" s="29" t="s">
         <v>319</v>
       </c>
-      <c r="K9" s="20"/>
-      <c r="L9" s="20"/>
+      <c r="K9" s="29"/>
+      <c r="L9" s="29"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="19"/>
-      <c r="B10" s="18" t="s">
-        <v>246</v>
-      </c>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20" t="s">
+      <c r="A10" s="28"/>
+      <c r="B10" s="20" t="s">
+        <v>246</v>
+      </c>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29" t="s">
         <v>248</v>
       </c>
       <c r="F10" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="20"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="29"/>
+      <c r="L10" s="29"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
@@ -1954,56 +1951,56 @@
       <c r="L11" s="8"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="B12" s="18" t="s">
-        <v>246</v>
-      </c>
-      <c r="C12" s="20" t="s">
+      <c r="B12" s="20" t="s">
+        <v>246</v>
+      </c>
+      <c r="C12" s="29" t="s">
         <v>144</v>
       </c>
-      <c r="D12" s="20" t="s">
+      <c r="D12" s="29" t="s">
         <v>199</v>
       </c>
-      <c r="E12" s="20" t="s">
+      <c r="E12" s="29" t="s">
         <v>248</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="G12" s="20" t="s">
+      <c r="G12" s="29" t="s">
         <v>310</v>
       </c>
-      <c r="H12" s="20" t="s">
+      <c r="H12" s="29" t="s">
         <v>251</v>
       </c>
-      <c r="I12" s="20" t="s">
+      <c r="I12" s="29" t="s">
         <v>305</v>
       </c>
-      <c r="J12" s="20" t="s">
+      <c r="J12" s="29" t="s">
         <v>319</v>
       </c>
-      <c r="K12" s="20"/>
-      <c r="L12" s="20"/>
+      <c r="K12" s="29"/>
+      <c r="L12" s="29"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="19"/>
-      <c r="B13" s="18" t="s">
-        <v>246</v>
-      </c>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
+      <c r="A13" s="28"/>
+      <c r="B13" s="20" t="s">
+        <v>246</v>
+      </c>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
       <c r="F13" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="20"/>
-      <c r="L13" s="20"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="29"/>
+      <c r="K13" s="29"/>
+      <c r="L13" s="29"/>
     </row>
     <row r="14" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
@@ -2040,1982 +2037,1986 @@
       <c r="L14" s="8"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="B15" s="18" t="s">
-        <v>246</v>
-      </c>
-      <c r="C15" s="20" t="s">
+      <c r="B15" s="20" t="s">
+        <v>246</v>
+      </c>
+      <c r="C15" s="29" t="s">
         <v>145</v>
       </c>
-      <c r="D15" s="20" t="s">
+      <c r="D15" s="29" t="s">
         <v>201</v>
       </c>
-      <c r="E15" s="20" t="s">
+      <c r="E15" s="29" t="s">
         <v>248</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="G15" s="20" t="s">
+      <c r="G15" s="29" t="s">
         <v>310</v>
       </c>
-      <c r="H15" s="20" t="s">
+      <c r="H15" s="29" t="s">
         <v>226</v>
       </c>
-      <c r="I15" s="20" t="s">
+      <c r="I15" s="29" t="s">
         <v>305</v>
       </c>
-      <c r="J15" s="20" t="s">
+      <c r="J15" s="29" t="s">
         <v>319</v>
       </c>
-      <c r="K15" s="20"/>
-      <c r="L15" s="20"/>
+      <c r="K15" s="29"/>
+      <c r="L15" s="29"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="19"/>
-      <c r="B16" s="18" t="s">
-        <v>246</v>
-      </c>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20" t="s">
+      <c r="A16" s="28"/>
+      <c r="B16" s="20" t="s">
+        <v>246</v>
+      </c>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29" t="s">
         <v>248</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="20"/>
-      <c r="L16" s="20"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="29"/>
+      <c r="L16" s="29"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A17" s="19" t="s">
+      <c r="A17" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="B17" s="18" t="s">
-        <v>246</v>
-      </c>
-      <c r="C17" s="20" t="s">
+      <c r="B17" s="20" t="s">
+        <v>246</v>
+      </c>
+      <c r="C17" s="29" t="s">
         <v>146</v>
       </c>
-      <c r="D17" s="20" t="s">
+      <c r="D17" s="29" t="s">
         <v>202</v>
       </c>
-      <c r="E17" s="20" t="s">
+      <c r="E17" s="29" t="s">
         <v>248</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="G17" s="20" t="s">
+      <c r="G17" s="29" t="s">
         <v>314</v>
       </c>
-      <c r="H17" s="20" t="s">
+      <c r="H17" s="29" t="s">
         <v>227</v>
       </c>
-      <c r="I17" s="20" t="s">
+      <c r="I17" s="29" t="s">
         <v>305</v>
       </c>
-      <c r="J17" s="20" t="s">
+      <c r="J17" s="29" t="s">
         <v>319</v>
       </c>
-      <c r="K17" s="20"/>
-      <c r="L17" s="20"/>
+      <c r="K17" s="29"/>
+      <c r="L17" s="29"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A18" s="19"/>
-      <c r="B18" s="18" t="s">
-        <v>246</v>
-      </c>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20" t="s">
+      <c r="A18" s="28"/>
+      <c r="B18" s="20" t="s">
+        <v>246</v>
+      </c>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29" t="s">
         <v>248</v>
       </c>
       <c r="F18" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="20"/>
-      <c r="J18" s="20"/>
-      <c r="K18" s="20"/>
-      <c r="L18" s="20"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
+      <c r="K18" s="29"/>
+      <c r="L18" s="29"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A19" s="19" t="s">
+      <c r="A19" s="28" t="s">
         <v>113</v>
       </c>
-      <c r="B19" s="18" t="s">
-        <v>246</v>
-      </c>
-      <c r="C19" s="20" t="s">
+      <c r="B19" s="20" t="s">
+        <v>246</v>
+      </c>
+      <c r="C19" s="29" t="s">
         <v>146</v>
       </c>
-      <c r="D19" s="18" t="s">
+      <c r="D19" s="20" t="s">
         <v>203</v>
       </c>
-      <c r="E19" s="18" t="s">
+      <c r="E19" s="20" t="s">
         <v>248</v>
       </c>
       <c r="F19" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="G19" s="20" t="s">
+      <c r="G19" s="29" t="s">
         <v>315</v>
       </c>
-      <c r="H19" s="18" t="s">
+      <c r="H19" s="20" t="s">
         <v>252</v>
       </c>
-      <c r="I19" s="18" t="s">
+      <c r="I19" s="20" t="s">
         <v>305</v>
       </c>
-      <c r="J19" s="18" t="s">
+      <c r="J19" s="20" t="s">
         <v>319</v>
       </c>
-      <c r="K19" s="18"/>
-      <c r="L19" s="18"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="19"/>
-      <c r="B20" s="18" t="s">
-        <v>246</v>
-      </c>
-      <c r="C20" s="20"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18" t="s">
+      <c r="A20" s="28"/>
+      <c r="B20" s="20" t="s">
+        <v>246</v>
+      </c>
+      <c r="C20" s="29"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20" t="s">
         <v>248</v>
       </c>
       <c r="F20" s="8" t="s">
         <v>219</v>
       </c>
-      <c r="G20" s="20"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="18"/>
-      <c r="L20" s="18"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="20"/>
+      <c r="L20" s="20"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A21" s="19" t="s">
+      <c r="A21" s="28" t="s">
         <v>118</v>
       </c>
-      <c r="B21" s="18" t="s">
-        <v>246</v>
-      </c>
-      <c r="C21" s="20" t="s">
+      <c r="B21" s="20" t="s">
+        <v>246</v>
+      </c>
+      <c r="C21" s="29" t="s">
         <v>147</v>
       </c>
-      <c r="D21" s="20" t="s">
+      <c r="D21" s="29" t="s">
         <v>204</v>
       </c>
-      <c r="E21" s="20" t="s">
+      <c r="E21" s="29" t="s">
         <v>248</v>
       </c>
       <c r="F21" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="G21" s="20" t="s">
+      <c r="G21" s="29" t="s">
         <v>310</v>
       </c>
-      <c r="H21" s="20" t="s">
+      <c r="H21" s="29" t="s">
         <v>253</v>
       </c>
-      <c r="I21" s="20" t="s">
+      <c r="I21" s="29" t="s">
         <v>305</v>
       </c>
-      <c r="J21" s="20" t="s">
+      <c r="J21" s="29" t="s">
         <v>319</v>
       </c>
-      <c r="K21" s="20"/>
-      <c r="L21" s="20"/>
+      <c r="K21" s="29"/>
+      <c r="L21" s="29"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A22" s="19"/>
-      <c r="B22" s="18" t="s">
-        <v>246</v>
-      </c>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
+      <c r="A22" s="28"/>
+      <c r="B22" s="20" t="s">
+        <v>246</v>
+      </c>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
       <c r="F22" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="20"/>
-      <c r="K22" s="20"/>
-      <c r="L22" s="20"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="29"/>
+      <c r="K22" s="29"/>
+      <c r="L22" s="29"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A23" s="25" t="s">
+      <c r="A23" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="B23" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C23" s="26" t="s">
+      <c r="B23" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C23" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="D23" s="23" t="s">
+      <c r="D23" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="E23" s="23" t="s">
+      <c r="E23" s="21" t="s">
         <v>248</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="G23" s="20" t="s">
+      <c r="G23" s="29" t="s">
         <v>310</v>
       </c>
-      <c r="H23" s="18" t="s">
+      <c r="H23" s="20" t="s">
         <v>254</v>
       </c>
-      <c r="I23" s="23" t="s">
+      <c r="I23" s="21" t="s">
         <v>305</v>
       </c>
-      <c r="J23" s="23" t="s">
+      <c r="J23" s="21" t="s">
         <v>319</v>
       </c>
-      <c r="K23" s="23"/>
-      <c r="L23" s="23"/>
+      <c r="K23" s="21"/>
+      <c r="L23" s="21"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A24" s="25"/>
-      <c r="B24" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C24" s="26"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="23"/>
+      <c r="A24" s="18"/>
+      <c r="B24" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C24" s="19"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
       <c r="F24" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="G24" s="20"/>
-      <c r="H24" s="18"/>
-      <c r="I24" s="23"/>
-      <c r="J24" s="23"/>
-      <c r="K24" s="23"/>
-      <c r="L24" s="23"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="21"/>
+      <c r="K24" s="21"/>
+      <c r="L24" s="21"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A25" s="25"/>
-      <c r="B25" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C25" s="26"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="23" t="s">
+      <c r="A25" s="18"/>
+      <c r="B25" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C25" s="19"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21" t="s">
         <v>248</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="G25" s="20"/>
-      <c r="H25" s="18"/>
-      <c r="I25" s="23"/>
-      <c r="J25" s="23"/>
-      <c r="K25" s="23"/>
-      <c r="L25" s="23"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="21"/>
+      <c r="K25" s="21"/>
+      <c r="L25" s="21"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A26" s="25"/>
-      <c r="B26" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C26" s="26"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="23"/>
+      <c r="A26" s="18"/>
+      <c r="B26" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C26" s="19"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
       <c r="F26" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="G26" s="20"/>
-      <c r="H26" s="18"/>
-      <c r="I26" s="23"/>
-      <c r="J26" s="23"/>
-      <c r="K26" s="23"/>
-      <c r="L26" s="23"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="21"/>
+      <c r="J26" s="21"/>
+      <c r="K26" s="21"/>
+      <c r="L26" s="21"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A27" s="25"/>
-      <c r="B27" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C27" s="26"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23" t="s">
+      <c r="A27" s="18"/>
+      <c r="B27" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C27" s="19"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21" t="s">
         <v>248</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="G27" s="20"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="23"/>
-      <c r="J27" s="23"/>
-      <c r="K27" s="23"/>
-      <c r="L27" s="23"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="21"/>
+      <c r="K27" s="21"/>
+      <c r="L27" s="21"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A28" s="25"/>
-      <c r="B28" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C28" s="26"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
+      <c r="A28" s="18"/>
+      <c r="B28" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C28" s="19"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
       <c r="F28" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="G28" s="20"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="23"/>
-      <c r="J28" s="23"/>
-      <c r="K28" s="23"/>
-      <c r="L28" s="23"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="21"/>
+      <c r="J28" s="21"/>
+      <c r="K28" s="21"/>
+      <c r="L28" s="21"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A29" s="25" t="s">
+      <c r="A29" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="B29" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C29" s="26" t="s">
+      <c r="B29" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C29" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="D29" s="21" t="s">
+      <c r="D29" s="22" t="s">
         <v>159</v>
       </c>
-      <c r="E29" s="21" t="s">
+      <c r="E29" s="22" t="s">
         <v>248</v>
       </c>
       <c r="F29" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="G29" s="32" t="s">
+      <c r="G29" s="30" t="s">
         <v>316</v>
       </c>
-      <c r="H29" s="21" t="s">
+      <c r="H29" s="22" t="s">
         <v>160</v>
       </c>
-      <c r="I29" s="23" t="s">
+      <c r="I29" s="21" t="s">
         <v>305</v>
       </c>
-      <c r="J29" s="23" t="s">
+      <c r="J29" s="21" t="s">
         <v>319</v>
       </c>
-      <c r="K29" s="23"/>
-      <c r="L29" s="23"/>
+      <c r="K29" s="21"/>
+      <c r="L29" s="21"/>
     </row>
     <row r="30" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A30" s="25"/>
-      <c r="B30" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C30" s="26"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
+      <c r="A30" s="18"/>
+      <c r="B30" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C30" s="19"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
       <c r="F30" s="8" t="s">
         <v>257</v>
       </c>
-      <c r="G30" s="32"/>
-      <c r="H30" s="21"/>
-      <c r="I30" s="23"/>
-      <c r="J30" s="23"/>
-      <c r="K30" s="23"/>
-      <c r="L30" s="23"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="22"/>
+      <c r="I30" s="21"/>
+      <c r="J30" s="21"/>
+      <c r="K30" s="21"/>
+      <c r="L30" s="21"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A31" s="25"/>
-      <c r="B31" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C31" s="26"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21" t="s">
+      <c r="A31" s="18"/>
+      <c r="B31" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C31" s="19"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="22" t="s">
         <v>248</v>
       </c>
       <c r="F31" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="G31" s="32"/>
-      <c r="H31" s="21"/>
-      <c r="I31" s="23"/>
-      <c r="J31" s="23"/>
-      <c r="K31" s="23"/>
-      <c r="L31" s="23"/>
+      <c r="G31" s="30"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="21"/>
+      <c r="J31" s="21"/>
+      <c r="K31" s="21"/>
+      <c r="L31" s="21"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A32" s="25"/>
-      <c r="B32" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C32" s="26"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="21"/>
+      <c r="A32" s="18"/>
+      <c r="B32" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C32" s="19"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="22"/>
       <c r="F32" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="G32" s="32"/>
-      <c r="H32" s="21"/>
-      <c r="I32" s="23"/>
-      <c r="J32" s="23"/>
-      <c r="K32" s="23"/>
-      <c r="L32" s="23"/>
+      <c r="G32" s="30"/>
+      <c r="H32" s="22"/>
+      <c r="I32" s="21"/>
+      <c r="J32" s="21"/>
+      <c r="K32" s="21"/>
+      <c r="L32" s="21"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A33" s="25" t="s">
+      <c r="A33" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="B33" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C33" s="26" t="s">
+      <c r="B33" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C33" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="D33" s="21" t="s">
+      <c r="D33" s="22" t="s">
         <v>164</v>
       </c>
-      <c r="E33" s="21"/>
+      <c r="E33" s="22"/>
       <c r="F33" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="G33" s="24" t="s">
+      <c r="G33" s="27" t="s">
         <v>310</v>
       </c>
-      <c r="H33" s="21" t="s">
+      <c r="H33" s="22" t="s">
         <v>167</v>
       </c>
-      <c r="I33" s="28" t="s">
+      <c r="I33" s="23" t="s">
         <v>305</v>
       </c>
-      <c r="J33" s="23" t="s">
+      <c r="J33" s="21" t="s">
         <v>319</v>
       </c>
-      <c r="K33" s="23"/>
-      <c r="L33" s="23"/>
+      <c r="K33" s="21"/>
+      <c r="L33" s="21"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A34" s="25"/>
-      <c r="B34" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C34" s="26"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="21" t="s">
+      <c r="A34" s="18"/>
+      <c r="B34" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C34" s="19"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="22" t="s">
         <v>248</v>
       </c>
       <c r="F34" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="G34" s="24"/>
-      <c r="H34" s="21"/>
-      <c r="I34" s="29"/>
-      <c r="J34" s="23"/>
-      <c r="K34" s="23"/>
-      <c r="L34" s="23"/>
+      <c r="G34" s="27"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="24"/>
+      <c r="J34" s="21"/>
+      <c r="K34" s="21"/>
+      <c r="L34" s="21"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A35" s="25"/>
-      <c r="B35" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C35" s="26"/>
-      <c r="D35" s="21"/>
-      <c r="E35" s="21"/>
+      <c r="A35" s="18"/>
+      <c r="B35" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C35" s="19"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
       <c r="F35" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="G35" s="24"/>
-      <c r="H35" s="21"/>
-      <c r="I35" s="30"/>
-      <c r="J35" s="23"/>
-      <c r="K35" s="23"/>
-      <c r="L35" s="23"/>
+      <c r="G35" s="27"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="25"/>
+      <c r="J35" s="21"/>
+      <c r="K35" s="21"/>
+      <c r="L35" s="21"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A36" s="25" t="s">
+      <c r="A36" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="B36" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C36" s="26" t="s">
+      <c r="B36" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C36" s="19" t="s">
         <v>168</v>
       </c>
-      <c r="D36" s="23" t="s">
+      <c r="D36" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="E36" s="23" t="s">
+      <c r="E36" s="21" t="s">
         <v>248</v>
       </c>
       <c r="F36" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="G36" s="26" t="s">
+      <c r="G36" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="H36" s="23" t="s">
+      <c r="H36" s="21" t="s">
         <v>171</v>
       </c>
-      <c r="I36" s="23" t="s">
+      <c r="I36" s="21" t="s">
         <v>305</v>
       </c>
-      <c r="J36" s="23" t="s">
+      <c r="J36" s="21" t="s">
         <v>319</v>
       </c>
-      <c r="K36" s="23"/>
-      <c r="L36" s="23"/>
+      <c r="K36" s="21"/>
+      <c r="L36" s="21"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A37" s="25"/>
-      <c r="B37" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C37" s="26"/>
-      <c r="D37" s="23"/>
-      <c r="E37" s="23"/>
+      <c r="A37" s="18"/>
+      <c r="B37" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C37" s="19"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="21"/>
       <c r="F37" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="G37" s="26"/>
-      <c r="H37" s="23"/>
-      <c r="I37" s="23"/>
-      <c r="J37" s="23"/>
-      <c r="K37" s="23"/>
-      <c r="L37" s="23"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="21"/>
+      <c r="I37" s="21"/>
+      <c r="J37" s="21"/>
+      <c r="K37" s="21"/>
+      <c r="L37" s="21"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A38" s="25"/>
-      <c r="B38" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C38" s="26"/>
-      <c r="D38" s="23"/>
-      <c r="E38" s="23" t="s">
+      <c r="A38" s="18"/>
+      <c r="B38" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C38" s="19"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="21" t="s">
         <v>248</v>
       </c>
       <c r="F38" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="G38" s="26"/>
-      <c r="H38" s="23"/>
-      <c r="I38" s="23"/>
-      <c r="J38" s="23"/>
-      <c r="K38" s="23"/>
-      <c r="L38" s="23"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="21"/>
+      <c r="I38" s="21"/>
+      <c r="J38" s="21"/>
+      <c r="K38" s="21"/>
+      <c r="L38" s="21"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A39" s="25"/>
-      <c r="B39" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C39" s="26"/>
-      <c r="D39" s="23"/>
-      <c r="E39" s="23"/>
+      <c r="A39" s="18"/>
+      <c r="B39" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C39" s="19"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="21"/>
       <c r="F39" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="G39" s="26"/>
-      <c r="H39" s="23"/>
-      <c r="I39" s="23"/>
-      <c r="J39" s="23"/>
-      <c r="K39" s="23"/>
-      <c r="L39" s="23"/>
+      <c r="G39" s="19"/>
+      <c r="H39" s="21"/>
+      <c r="I39" s="21"/>
+      <c r="J39" s="21"/>
+      <c r="K39" s="21"/>
+      <c r="L39" s="21"/>
     </row>
     <row r="40" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="22" t="s">
+      <c r="A40" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="B40" s="21" t="s">
-        <v>246</v>
-      </c>
-      <c r="C40" s="24" t="s">
+      <c r="B40" s="22" t="s">
+        <v>246</v>
+      </c>
+      <c r="C40" s="27" t="s">
         <v>172</v>
       </c>
-      <c r="D40" s="21" t="s">
+      <c r="D40" s="22" t="s">
         <v>173</v>
       </c>
-      <c r="E40" s="21" t="s">
+      <c r="E40" s="22" t="s">
         <v>248</v>
       </c>
       <c r="F40" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="G40" s="24" t="s">
+      <c r="G40" s="27" t="s">
         <v>310</v>
       </c>
-      <c r="H40" s="21" t="s">
+      <c r="H40" s="22" t="s">
         <v>175</v>
       </c>
-      <c r="I40" s="21" t="s">
+      <c r="I40" s="22" t="s">
         <v>305</v>
       </c>
-      <c r="J40" s="21" t="s">
+      <c r="J40" s="22" t="s">
         <v>319</v>
       </c>
-      <c r="K40" s="21"/>
-      <c r="L40" s="21"/>
+      <c r="K40" s="22"/>
+      <c r="L40" s="22"/>
     </row>
     <row r="41" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="22"/>
-      <c r="B41" s="21" t="s">
-        <v>246</v>
-      </c>
-      <c r="C41" s="24"/>
-      <c r="D41" s="21"/>
-      <c r="E41" s="21"/>
+      <c r="A41" s="26"/>
+      <c r="B41" s="22" t="s">
+        <v>246</v>
+      </c>
+      <c r="C41" s="27"/>
+      <c r="D41" s="22"/>
+      <c r="E41" s="22"/>
       <c r="F41" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="G41" s="24"/>
-      <c r="H41" s="21"/>
-      <c r="I41" s="21"/>
-      <c r="J41" s="21"/>
-      <c r="K41" s="21"/>
-      <c r="L41" s="21"/>
+      <c r="G41" s="27"/>
+      <c r="H41" s="22"/>
+      <c r="I41" s="22"/>
+      <c r="J41" s="22"/>
+      <c r="K41" s="22"/>
+      <c r="L41" s="22"/>
     </row>
     <row r="42" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="22"/>
-      <c r="B42" s="21" t="s">
-        <v>246</v>
-      </c>
-      <c r="C42" s="24"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="21" t="s">
+      <c r="A42" s="26"/>
+      <c r="B42" s="22" t="s">
+        <v>246</v>
+      </c>
+      <c r="C42" s="27"/>
+      <c r="D42" s="22"/>
+      <c r="E42" s="22" t="s">
         <v>248</v>
       </c>
       <c r="F42" s="13" t="s">
         <v>157</v>
       </c>
-      <c r="G42" s="24"/>
-      <c r="H42" s="21"/>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21"/>
-      <c r="K42" s="21"/>
-      <c r="L42" s="21"/>
+      <c r="G42" s="27"/>
+      <c r="H42" s="22"/>
+      <c r="I42" s="22"/>
+      <c r="J42" s="22"/>
+      <c r="K42" s="22"/>
+      <c r="L42" s="22"/>
     </row>
     <row r="43" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="22"/>
-      <c r="B43" s="21" t="s">
-        <v>246</v>
-      </c>
-      <c r="C43" s="24"/>
-      <c r="D43" s="21"/>
-      <c r="E43" s="21"/>
+      <c r="A43" s="26"/>
+      <c r="B43" s="22" t="s">
+        <v>246</v>
+      </c>
+      <c r="C43" s="27"/>
+      <c r="D43" s="22"/>
+      <c r="E43" s="22"/>
       <c r="F43" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="G43" s="24"/>
-      <c r="H43" s="21"/>
-      <c r="I43" s="21"/>
-      <c r="J43" s="21"/>
-      <c r="K43" s="21"/>
-      <c r="L43" s="21"/>
+      <c r="G43" s="27"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
+      <c r="K43" s="22"/>
+      <c r="L43" s="22"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A44" s="22" t="s">
+      <c r="A44" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="B44" s="21" t="s">
-        <v>246</v>
-      </c>
-      <c r="C44" s="24" t="s">
+      <c r="B44" s="22" t="s">
+        <v>246</v>
+      </c>
+      <c r="C44" s="27" t="s">
         <v>176</v>
       </c>
-      <c r="D44" s="20" t="s">
+      <c r="D44" s="29" t="s">
         <v>177</v>
       </c>
-      <c r="E44" s="21" t="s">
+      <c r="E44" s="22" t="s">
         <v>248</v>
       </c>
       <c r="F44" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="G44" s="20" t="s">
+      <c r="G44" s="29" t="s">
         <v>310</v>
       </c>
-      <c r="H44" s="18" t="s">
+      <c r="H44" s="20" t="s">
         <v>179</v>
       </c>
-      <c r="I44" s="18" t="s">
+      <c r="I44" s="20" t="s">
         <v>305</v>
       </c>
-      <c r="J44" s="18" t="s">
+      <c r="J44" s="20" t="s">
         <v>319</v>
       </c>
-      <c r="K44" s="18"/>
-      <c r="L44" s="18"/>
+      <c r="K44" s="20"/>
+      <c r="L44" s="20"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A45" s="22"/>
-      <c r="B45" s="21"/>
-      <c r="C45" s="24"/>
-      <c r="D45" s="20"/>
-      <c r="E45" s="21"/>
+      <c r="A45" s="26"/>
+      <c r="B45" s="22"/>
+      <c r="C45" s="27"/>
+      <c r="D45" s="29"/>
+      <c r="E45" s="22"/>
       <c r="F45" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="G45" s="20"/>
-      <c r="H45" s="18"/>
-      <c r="I45" s="18"/>
-      <c r="J45" s="18"/>
-      <c r="K45" s="18"/>
-      <c r="L45" s="18"/>
+      <c r="G45" s="29"/>
+      <c r="H45" s="20"/>
+      <c r="I45" s="20"/>
+      <c r="J45" s="20"/>
+      <c r="K45" s="20"/>
+      <c r="L45" s="20"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A46" s="22"/>
-      <c r="B46" s="21"/>
-      <c r="C46" s="24"/>
-      <c r="D46" s="20"/>
-      <c r="E46" s="21"/>
+      <c r="A46" s="26"/>
+      <c r="B46" s="22"/>
+      <c r="C46" s="27"/>
+      <c r="D46" s="29"/>
+      <c r="E46" s="22"/>
       <c r="F46" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="G46" s="20"/>
-      <c r="H46" s="18"/>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
-      <c r="K46" s="18"/>
-      <c r="L46" s="18"/>
+      <c r="G46" s="29"/>
+      <c r="H46" s="20"/>
+      <c r="I46" s="20"/>
+      <c r="J46" s="20"/>
+      <c r="K46" s="20"/>
+      <c r="L46" s="20"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A47" s="19" t="s">
+      <c r="A47" s="28" t="s">
         <v>136</v>
       </c>
-      <c r="B47" s="21" t="s">
-        <v>246</v>
-      </c>
-      <c r="C47" s="20" t="s">
+      <c r="B47" s="22" t="s">
+        <v>246</v>
+      </c>
+      <c r="C47" s="29" t="s">
         <v>181</v>
       </c>
-      <c r="D47" s="20" t="s">
+      <c r="D47" s="29" t="s">
         <v>182</v>
       </c>
-      <c r="E47" s="20" t="s">
+      <c r="E47" s="29" t="s">
         <v>248</v>
       </c>
       <c r="F47" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="G47" s="20" t="s">
+      <c r="G47" s="29" t="s">
         <v>310</v>
       </c>
-      <c r="H47" s="18" t="s">
+      <c r="H47" s="20" t="s">
         <v>307</v>
       </c>
-      <c r="I47" s="18" t="s">
+      <c r="I47" s="20" t="s">
         <v>306</v>
       </c>
-      <c r="J47" s="18" t="s">
+      <c r="J47" s="20" t="s">
         <v>319</v>
       </c>
-      <c r="K47" s="18"/>
-      <c r="L47" s="18"/>
+      <c r="K47" s="20"/>
+      <c r="L47" s="20"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A48" s="19"/>
-      <c r="B48" s="21"/>
-      <c r="C48" s="20"/>
-      <c r="D48" s="20"/>
-      <c r="E48" s="20"/>
+      <c r="A48" s="28"/>
+      <c r="B48" s="22"/>
+      <c r="C48" s="29"/>
+      <c r="D48" s="29"/>
+      <c r="E48" s="29"/>
       <c r="F48" s="8" t="s">
         <v>259</v>
       </c>
-      <c r="G48" s="20"/>
-      <c r="H48" s="18"/>
-      <c r="I48" s="18"/>
-      <c r="J48" s="18"/>
-      <c r="K48" s="18"/>
-      <c r="L48" s="18"/>
+      <c r="G48" s="29"/>
+      <c r="H48" s="20"/>
+      <c r="I48" s="20"/>
+      <c r="J48" s="20"/>
+      <c r="K48" s="20"/>
+      <c r="L48" s="20"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A49" s="19"/>
-      <c r="B49" s="21"/>
-      <c r="C49" s="20"/>
-      <c r="D49" s="20"/>
-      <c r="E49" s="20"/>
+      <c r="A49" s="28"/>
+      <c r="B49" s="22"/>
+      <c r="C49" s="29"/>
+      <c r="D49" s="29"/>
+      <c r="E49" s="29"/>
       <c r="F49" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="G49" s="20"/>
-      <c r="H49" s="18"/>
-      <c r="I49" s="18"/>
-      <c r="J49" s="18"/>
-      <c r="K49" s="18"/>
-      <c r="L49" s="18"/>
+      <c r="G49" s="29"/>
+      <c r="H49" s="20"/>
+      <c r="I49" s="20"/>
+      <c r="J49" s="20"/>
+      <c r="K49" s="20"/>
+      <c r="L49" s="20"/>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A50" s="19"/>
-      <c r="B50" s="21"/>
-      <c r="C50" s="20"/>
-      <c r="D50" s="20"/>
-      <c r="E50" s="20"/>
+      <c r="A50" s="28"/>
+      <c r="B50" s="22"/>
+      <c r="C50" s="29"/>
+      <c r="D50" s="29"/>
+      <c r="E50" s="29"/>
       <c r="F50" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="G50" s="20"/>
-      <c r="H50" s="18"/>
-      <c r="I50" s="18"/>
-      <c r="J50" s="18"/>
-      <c r="K50" s="18"/>
-      <c r="L50" s="18"/>
+      <c r="G50" s="29"/>
+      <c r="H50" s="20"/>
+      <c r="I50" s="20"/>
+      <c r="J50" s="20"/>
+      <c r="K50" s="20"/>
+      <c r="L50" s="20"/>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A51" s="19" t="s">
+      <c r="A51" s="28" t="s">
         <v>229</v>
       </c>
-      <c r="B51" s="18" t="s">
-        <v>246</v>
-      </c>
-      <c r="C51" s="20" t="s">
+      <c r="B51" s="20" t="s">
+        <v>246</v>
+      </c>
+      <c r="C51" s="29" t="s">
         <v>183</v>
       </c>
-      <c r="D51" s="20" t="s">
+      <c r="D51" s="29" t="s">
         <v>184</v>
       </c>
-      <c r="E51" s="20" t="s">
+      <c r="E51" s="29" t="s">
         <v>248</v>
       </c>
       <c r="F51" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="G51" s="20" t="s">
+      <c r="G51" s="29" t="s">
         <v>310</v>
       </c>
-      <c r="H51" s="18" t="s">
+      <c r="H51" s="20" t="s">
         <v>308</v>
       </c>
-      <c r="I51" s="18" t="s">
+      <c r="I51" s="20" t="s">
         <v>261</v>
       </c>
-      <c r="J51" s="18" t="s">
+      <c r="J51" s="20" t="s">
         <v>319</v>
       </c>
-      <c r="K51" s="18"/>
-      <c r="L51" s="18"/>
+      <c r="K51" s="20"/>
+      <c r="L51" s="20"/>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A52" s="19"/>
-      <c r="B52" s="18"/>
-      <c r="C52" s="20"/>
-      <c r="D52" s="20"/>
-      <c r="E52" s="20"/>
+      <c r="A52" s="28"/>
+      <c r="B52" s="20"/>
+      <c r="C52" s="29"/>
+      <c r="D52" s="29"/>
+      <c r="E52" s="29"/>
       <c r="F52" s="8" t="s">
         <v>258</v>
       </c>
-      <c r="G52" s="20"/>
-      <c r="H52" s="18"/>
-      <c r="I52" s="18"/>
-      <c r="J52" s="18"/>
-      <c r="K52" s="18"/>
-      <c r="L52" s="18"/>
+      <c r="G52" s="29"/>
+      <c r="H52" s="20"/>
+      <c r="I52" s="20"/>
+      <c r="J52" s="20"/>
+      <c r="K52" s="20"/>
+      <c r="L52" s="20"/>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A53" s="19"/>
-      <c r="B53" s="18"/>
-      <c r="C53" s="20"/>
-      <c r="D53" s="20"/>
-      <c r="E53" s="20"/>
+      <c r="A53" s="28"/>
+      <c r="B53" s="20"/>
+      <c r="C53" s="29"/>
+      <c r="D53" s="29"/>
+      <c r="E53" s="29"/>
       <c r="F53" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="G53" s="20"/>
-      <c r="H53" s="18"/>
-      <c r="I53" s="18"/>
-      <c r="J53" s="18"/>
-      <c r="K53" s="18"/>
-      <c r="L53" s="18"/>
+      <c r="G53" s="29"/>
+      <c r="H53" s="20"/>
+      <c r="I53" s="20"/>
+      <c r="J53" s="20"/>
+      <c r="K53" s="20"/>
+      <c r="L53" s="20"/>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A54" s="19"/>
-      <c r="B54" s="18"/>
-      <c r="C54" s="20"/>
-      <c r="D54" s="20"/>
-      <c r="E54" s="20"/>
+      <c r="A54" s="28"/>
+      <c r="B54" s="20"/>
+      <c r="C54" s="29"/>
+      <c r="D54" s="29"/>
+      <c r="E54" s="29"/>
       <c r="F54" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="G54" s="20"/>
-      <c r="H54" s="18"/>
-      <c r="I54" s="18"/>
-      <c r="J54" s="18"/>
-      <c r="K54" s="18"/>
-      <c r="L54" s="18"/>
+      <c r="G54" s="29"/>
+      <c r="H54" s="20"/>
+      <c r="I54" s="20"/>
+      <c r="J54" s="20"/>
+      <c r="K54" s="20"/>
+      <c r="L54" s="20"/>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A55" s="19" t="s">
+      <c r="A55" s="28" t="s">
         <v>230</v>
       </c>
-      <c r="B55" s="18" t="s">
-        <v>246</v>
-      </c>
-      <c r="C55" s="20" t="s">
+      <c r="B55" s="20" t="s">
+        <v>246</v>
+      </c>
+      <c r="C55" s="29" t="s">
         <v>186</v>
       </c>
-      <c r="D55" s="20" t="s">
+      <c r="D55" s="29" t="s">
         <v>187</v>
       </c>
-      <c r="E55" s="20" t="s">
+      <c r="E55" s="29" t="s">
         <v>248</v>
       </c>
       <c r="F55" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="G55" s="20" t="s">
+      <c r="G55" s="29" t="s">
         <v>310</v>
       </c>
-      <c r="H55" s="18" t="s">
+      <c r="H55" s="20" t="s">
         <v>190</v>
       </c>
-      <c r="I55" s="18" t="s">
+      <c r="I55" s="20" t="s">
         <v>305</v>
       </c>
-      <c r="J55" s="18" t="s">
+      <c r="J55" s="20" t="s">
         <v>319</v>
       </c>
-      <c r="K55" s="18"/>
-      <c r="L55" s="18"/>
+      <c r="K55" s="20"/>
+      <c r="L55" s="20"/>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A56" s="19"/>
-      <c r="B56" s="18"/>
-      <c r="C56" s="20"/>
-      <c r="D56" s="20"/>
-      <c r="E56" s="20"/>
+      <c r="A56" s="28"/>
+      <c r="B56" s="20"/>
+      <c r="C56" s="29"/>
+      <c r="D56" s="29"/>
+      <c r="E56" s="29"/>
       <c r="F56" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="G56" s="20"/>
-      <c r="H56" s="18"/>
-      <c r="I56" s="18"/>
-      <c r="J56" s="18"/>
-      <c r="K56" s="18"/>
-      <c r="L56" s="18"/>
+      <c r="G56" s="29"/>
+      <c r="H56" s="20"/>
+      <c r="I56" s="20"/>
+      <c r="J56" s="20"/>
+      <c r="K56" s="20"/>
+      <c r="L56" s="20"/>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A57" s="19"/>
-      <c r="B57" s="18"/>
-      <c r="C57" s="20"/>
-      <c r="D57" s="20"/>
-      <c r="E57" s="20"/>
+      <c r="A57" s="28"/>
+      <c r="B57" s="20"/>
+      <c r="C57" s="29"/>
+      <c r="D57" s="29"/>
+      <c r="E57" s="29"/>
       <c r="F57" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="G57" s="20"/>
-      <c r="H57" s="18"/>
-      <c r="I57" s="18"/>
-      <c r="J57" s="18"/>
-      <c r="K57" s="18"/>
-      <c r="L57" s="18"/>
+      <c r="G57" s="29"/>
+      <c r="H57" s="20"/>
+      <c r="I57" s="20"/>
+      <c r="J57" s="20"/>
+      <c r="K57" s="20"/>
+      <c r="L57" s="20"/>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A58" s="25" t="s">
+      <c r="A58" s="18" t="s">
         <v>231</v>
       </c>
-      <c r="B58" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C58" s="26" t="s">
+      <c r="B58" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C58" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="D58" s="23" t="s">
+      <c r="D58" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="E58" s="23" t="s">
+      <c r="E58" s="21" t="s">
         <v>248</v>
       </c>
       <c r="F58" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="G58" s="26" t="s">
+      <c r="G58" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="H58" s="23" t="s">
+      <c r="H58" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="I58" s="23" t="s">
+      <c r="I58" s="21" t="s">
         <v>305</v>
       </c>
-      <c r="J58" s="23" t="s">
+      <c r="J58" s="21" t="s">
         <v>319</v>
       </c>
-      <c r="K58" s="23"/>
-      <c r="L58" s="23"/>
+      <c r="K58" s="21"/>
+      <c r="L58" s="21"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A59" s="25"/>
-      <c r="B59" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C59" s="26"/>
-      <c r="D59" s="23"/>
-      <c r="E59" s="23"/>
+      <c r="A59" s="18"/>
+      <c r="B59" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C59" s="19"/>
+      <c r="D59" s="21"/>
+      <c r="E59" s="21"/>
       <c r="F59" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="G59" s="26"/>
-      <c r="H59" s="23"/>
-      <c r="I59" s="23"/>
-      <c r="J59" s="23"/>
-      <c r="K59" s="23"/>
-      <c r="L59" s="23"/>
+      <c r="G59" s="19"/>
+      <c r="H59" s="21"/>
+      <c r="I59" s="21"/>
+      <c r="J59" s="21"/>
+      <c r="K59" s="21"/>
+      <c r="L59" s="21"/>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A60" s="25"/>
-      <c r="B60" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C60" s="26"/>
-      <c r="D60" s="23"/>
-      <c r="E60" s="23" t="s">
+      <c r="A60" s="18"/>
+      <c r="B60" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C60" s="19"/>
+      <c r="D60" s="21"/>
+      <c r="E60" s="21" t="s">
         <v>248</v>
       </c>
       <c r="F60" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="G60" s="26"/>
-      <c r="H60" s="23"/>
-      <c r="I60" s="23"/>
-      <c r="J60" s="23"/>
-      <c r="K60" s="23"/>
-      <c r="L60" s="23"/>
+      <c r="G60" s="19"/>
+      <c r="H60" s="21"/>
+      <c r="I60" s="21"/>
+      <c r="J60" s="21"/>
+      <c r="K60" s="21"/>
+      <c r="L60" s="21"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A61" s="25"/>
-      <c r="B61" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C61" s="26"/>
-      <c r="D61" s="23"/>
-      <c r="E61" s="23"/>
+      <c r="A61" s="18"/>
+      <c r="B61" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C61" s="19"/>
+      <c r="D61" s="21"/>
+      <c r="E61" s="21"/>
       <c r="F61" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="G61" s="26"/>
-      <c r="H61" s="23"/>
-      <c r="I61" s="23"/>
-      <c r="J61" s="23"/>
-      <c r="K61" s="23"/>
-      <c r="L61" s="23"/>
+      <c r="G61" s="19"/>
+      <c r="H61" s="21"/>
+      <c r="I61" s="21"/>
+      <c r="J61" s="21"/>
+      <c r="K61" s="21"/>
+      <c r="L61" s="21"/>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A62" s="25" t="s">
+      <c r="A62" s="18" t="s">
         <v>232</v>
       </c>
-      <c r="B62" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C62" s="26" t="s">
+      <c r="B62" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C62" s="19" t="s">
         <v>191</v>
       </c>
-      <c r="D62" s="23" t="s">
+      <c r="D62" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="E62" s="23" t="s">
+      <c r="E62" s="21" t="s">
         <v>248</v>
       </c>
       <c r="F62" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="G62" s="26" t="s">
+      <c r="G62" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="H62" s="23" t="s">
+      <c r="H62" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="I62" s="23" t="s">
+      <c r="I62" s="21" t="s">
         <v>305</v>
       </c>
-      <c r="J62" s="23" t="s">
+      <c r="J62" s="21" t="s">
         <v>319</v>
       </c>
-      <c r="K62" s="23"/>
-      <c r="L62" s="23"/>
+      <c r="K62" s="21"/>
+      <c r="L62" s="21"/>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A63" s="25"/>
-      <c r="B63" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C63" s="26"/>
-      <c r="D63" s="23"/>
-      <c r="E63" s="23" t="s">
+      <c r="A63" s="18"/>
+      <c r="B63" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C63" s="19"/>
+      <c r="D63" s="21"/>
+      <c r="E63" s="21" t="s">
         <v>248</v>
       </c>
       <c r="F63" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="G63" s="26"/>
-      <c r="H63" s="23"/>
-      <c r="I63" s="23"/>
-      <c r="J63" s="23"/>
-      <c r="K63" s="23"/>
-      <c r="L63" s="23"/>
+      <c r="G63" s="19"/>
+      <c r="H63" s="21"/>
+      <c r="I63" s="21"/>
+      <c r="J63" s="21"/>
+      <c r="K63" s="21"/>
+      <c r="L63" s="21"/>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A64" s="25"/>
-      <c r="B64" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C64" s="26"/>
-      <c r="D64" s="23"/>
-      <c r="E64" s="23"/>
+      <c r="A64" s="18"/>
+      <c r="B64" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C64" s="19"/>
+      <c r="D64" s="21"/>
+      <c r="E64" s="21"/>
       <c r="F64" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="G64" s="26"/>
-      <c r="H64" s="23"/>
-      <c r="I64" s="23"/>
-      <c r="J64" s="23"/>
-      <c r="K64" s="23"/>
-      <c r="L64" s="23"/>
+      <c r="G64" s="19"/>
+      <c r="H64" s="21"/>
+      <c r="I64" s="21"/>
+      <c r="J64" s="21"/>
+      <c r="K64" s="21"/>
+      <c r="L64" s="21"/>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A65" s="25"/>
-      <c r="B65" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C65" s="26"/>
-      <c r="D65" s="23"/>
-      <c r="E65" s="23" t="s">
+      <c r="A65" s="18"/>
+      <c r="B65" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C65" s="19"/>
+      <c r="D65" s="21"/>
+      <c r="E65" s="21" t="s">
         <v>248</v>
       </c>
       <c r="F65" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="G65" s="26"/>
-      <c r="H65" s="23"/>
-      <c r="I65" s="23"/>
-      <c r="J65" s="23"/>
-      <c r="K65" s="23"/>
-      <c r="L65" s="23"/>
+      <c r="G65" s="19"/>
+      <c r="H65" s="21"/>
+      <c r="I65" s="21"/>
+      <c r="J65" s="21"/>
+      <c r="K65" s="21"/>
+      <c r="L65" s="21"/>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A66" s="25" t="s">
+      <c r="A66" s="18" t="s">
         <v>233</v>
       </c>
-      <c r="B66" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C66" s="26" t="s">
+      <c r="B66" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C66" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="D66" s="23" t="s">
+      <c r="D66" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="E66" s="23" t="s">
+      <c r="E66" s="21" t="s">
         <v>248</v>
       </c>
       <c r="F66" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="G66" s="26" t="s">
+      <c r="G66" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="H66" s="23" t="s">
+      <c r="H66" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="I66" s="23" t="s">
+      <c r="I66" s="21" t="s">
         <v>305</v>
       </c>
-      <c r="J66" s="23" t="s">
+      <c r="J66" s="21" t="s">
         <v>319</v>
       </c>
-      <c r="K66" s="23"/>
-      <c r="L66" s="23"/>
+      <c r="K66" s="21"/>
+      <c r="L66" s="21"/>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A67" s="25"/>
-      <c r="B67" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C67" s="26"/>
-      <c r="D67" s="23"/>
-      <c r="E67" s="23" t="s">
+      <c r="A67" s="18"/>
+      <c r="B67" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C67" s="19"/>
+      <c r="D67" s="21"/>
+      <c r="E67" s="21" t="s">
         <v>248</v>
       </c>
       <c r="F67" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="G67" s="26"/>
-      <c r="H67" s="23"/>
-      <c r="I67" s="23"/>
-      <c r="J67" s="23"/>
-      <c r="K67" s="23"/>
-      <c r="L67" s="23"/>
+      <c r="G67" s="19"/>
+      <c r="H67" s="21"/>
+      <c r="I67" s="21"/>
+      <c r="J67" s="21"/>
+      <c r="K67" s="21"/>
+      <c r="L67" s="21"/>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A68" s="25"/>
-      <c r="B68" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C68" s="26"/>
-      <c r="D68" s="23"/>
-      <c r="E68" s="23"/>
+      <c r="A68" s="18"/>
+      <c r="B68" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C68" s="19"/>
+      <c r="D68" s="21"/>
+      <c r="E68" s="21"/>
       <c r="F68" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="G68" s="26"/>
-      <c r="H68" s="23"/>
-      <c r="I68" s="23"/>
-      <c r="J68" s="23"/>
-      <c r="K68" s="23"/>
-      <c r="L68" s="23"/>
+      <c r="G68" s="19"/>
+      <c r="H68" s="21"/>
+      <c r="I68" s="21"/>
+      <c r="J68" s="21"/>
+      <c r="K68" s="21"/>
+      <c r="L68" s="21"/>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A69" s="25"/>
-      <c r="B69" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C69" s="26"/>
-      <c r="D69" s="23"/>
-      <c r="E69" s="23" t="s">
+      <c r="A69" s="18"/>
+      <c r="B69" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C69" s="19"/>
+      <c r="D69" s="21"/>
+      <c r="E69" s="21" t="s">
         <v>248</v>
       </c>
       <c r="F69" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="G69" s="26"/>
-      <c r="H69" s="23"/>
-      <c r="I69" s="23"/>
-      <c r="J69" s="23"/>
-      <c r="K69" s="23"/>
-      <c r="L69" s="23"/>
+      <c r="G69" s="19"/>
+      <c r="H69" s="21"/>
+      <c r="I69" s="21"/>
+      <c r="J69" s="21"/>
+      <c r="K69" s="21"/>
+      <c r="L69" s="21"/>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A70" s="25" t="s">
+      <c r="A70" s="18" t="s">
         <v>234</v>
       </c>
-      <c r="B70" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C70" s="26" t="s">
+      <c r="B70" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C70" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="D70" s="23" t="s">
+      <c r="D70" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="E70" s="23" t="s">
+      <c r="E70" s="21" t="s">
         <v>248</v>
       </c>
       <c r="F70" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="G70" s="26" t="s">
+      <c r="G70" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="H70" s="23" t="s">
+      <c r="H70" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="I70" s="23" t="s">
+      <c r="I70" s="21" t="s">
         <v>305</v>
       </c>
-      <c r="J70" s="23" t="s">
+      <c r="J70" s="21" t="s">
         <v>319</v>
       </c>
-      <c r="K70" s="23"/>
-      <c r="L70" s="23"/>
+      <c r="K70" s="21"/>
+      <c r="L70" s="21"/>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A71" s="25"/>
-      <c r="B71" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C71" s="26"/>
-      <c r="D71" s="23"/>
-      <c r="E71" s="23" t="s">
+      <c r="A71" s="18"/>
+      <c r="B71" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C71" s="19"/>
+      <c r="D71" s="21"/>
+      <c r="E71" s="21" t="s">
         <v>248</v>
       </c>
       <c r="F71" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="G71" s="26"/>
-      <c r="H71" s="23"/>
-      <c r="I71" s="23"/>
-      <c r="J71" s="23"/>
-      <c r="K71" s="23"/>
-      <c r="L71" s="23"/>
+      <c r="G71" s="19"/>
+      <c r="H71" s="21"/>
+      <c r="I71" s="21"/>
+      <c r="J71" s="21"/>
+      <c r="K71" s="21"/>
+      <c r="L71" s="21"/>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A72" s="25"/>
-      <c r="B72" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C72" s="26"/>
-      <c r="D72" s="23"/>
-      <c r="E72" s="23"/>
+      <c r="A72" s="18"/>
+      <c r="B72" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C72" s="19"/>
+      <c r="D72" s="21"/>
+      <c r="E72" s="21"/>
       <c r="F72" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="G72" s="26"/>
-      <c r="H72" s="23"/>
-      <c r="I72" s="23"/>
-      <c r="J72" s="23"/>
-      <c r="K72" s="23"/>
-      <c r="L72" s="23"/>
+      <c r="G72" s="19"/>
+      <c r="H72" s="21"/>
+      <c r="I72" s="21"/>
+      <c r="J72" s="21"/>
+      <c r="K72" s="21"/>
+      <c r="L72" s="21"/>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A73" s="25"/>
-      <c r="B73" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C73" s="26"/>
-      <c r="D73" s="23"/>
-      <c r="E73" s="23" t="s">
+      <c r="A73" s="18"/>
+      <c r="B73" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C73" s="19"/>
+      <c r="D73" s="21"/>
+      <c r="E73" s="21" t="s">
         <v>248</v>
       </c>
       <c r="F73" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="G73" s="26"/>
-      <c r="H73" s="23"/>
-      <c r="I73" s="23"/>
-      <c r="J73" s="23"/>
-      <c r="K73" s="23"/>
-      <c r="L73" s="23"/>
+      <c r="G73" s="19"/>
+      <c r="H73" s="21"/>
+      <c r="I73" s="21"/>
+      <c r="J73" s="21"/>
+      <c r="K73" s="21"/>
+      <c r="L73" s="21"/>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A74" s="25"/>
-      <c r="B74" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C74" s="26"/>
-      <c r="D74" s="23"/>
-      <c r="E74" s="23"/>
+      <c r="A74" s="18"/>
+      <c r="B74" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C74" s="19"/>
+      <c r="D74" s="21"/>
+      <c r="E74" s="21"/>
       <c r="F74" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="G74" s="26"/>
-      <c r="H74" s="23"/>
-      <c r="I74" s="23"/>
-      <c r="J74" s="23"/>
-      <c r="K74" s="23"/>
-      <c r="L74" s="23"/>
+      <c r="G74" s="19"/>
+      <c r="H74" s="21"/>
+      <c r="I74" s="21"/>
+      <c r="J74" s="21"/>
+      <c r="K74" s="21"/>
+      <c r="L74" s="21"/>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A75" s="25" t="s">
+      <c r="A75" s="18" t="s">
         <v>235</v>
       </c>
-      <c r="B75" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C75" s="26" t="s">
+      <c r="B75" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C75" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="D75" s="23" t="s">
+      <c r="D75" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="E75" s="23" t="s">
+      <c r="E75" s="21" t="s">
         <v>248</v>
       </c>
       <c r="F75" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="G75" s="26" t="s">
+      <c r="G75" s="19" t="s">
         <v>317</v>
       </c>
-      <c r="H75" s="23" t="s">
+      <c r="H75" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="I75" s="23" t="s">
+      <c r="I75" s="21" t="s">
         <v>309</v>
       </c>
-      <c r="J75" s="23" t="s">
+      <c r="J75" s="21" t="s">
         <v>320</v>
       </c>
-      <c r="K75" s="23"/>
-      <c r="L75" s="23"/>
+      <c r="K75" s="21"/>
+      <c r="L75" s="21"/>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A76" s="25"/>
-      <c r="B76" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C76" s="26"/>
-      <c r="D76" s="23"/>
-      <c r="E76" s="23"/>
+      <c r="A76" s="18"/>
+      <c r="B76" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C76" s="19"/>
+      <c r="D76" s="21"/>
+      <c r="E76" s="21"/>
       <c r="F76" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="G76" s="26"/>
-      <c r="H76" s="23"/>
-      <c r="I76" s="23"/>
-      <c r="J76" s="23"/>
-      <c r="K76" s="23"/>
-      <c r="L76" s="23"/>
+      <c r="G76" s="19"/>
+      <c r="H76" s="21"/>
+      <c r="I76" s="21"/>
+      <c r="J76" s="21"/>
+      <c r="K76" s="21"/>
+      <c r="L76" s="21"/>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A77" s="25"/>
-      <c r="B77" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C77" s="26"/>
-      <c r="D77" s="23"/>
-      <c r="E77" s="23" t="s">
+      <c r="A77" s="18"/>
+      <c r="B77" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C77" s="19"/>
+      <c r="D77" s="21"/>
+      <c r="E77" s="21" t="s">
         <v>248</v>
       </c>
       <c r="F77" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="G77" s="26"/>
-      <c r="H77" s="23"/>
-      <c r="I77" s="23"/>
-      <c r="J77" s="23"/>
-      <c r="K77" s="23"/>
-      <c r="L77" s="23"/>
+      <c r="G77" s="19"/>
+      <c r="H77" s="21"/>
+      <c r="I77" s="21"/>
+      <c r="J77" s="21"/>
+      <c r="K77" s="21"/>
+      <c r="L77" s="21"/>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A78" s="25"/>
-      <c r="B78" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C78" s="26"/>
-      <c r="D78" s="23"/>
-      <c r="E78" s="23"/>
+      <c r="A78" s="18"/>
+      <c r="B78" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C78" s="19"/>
+      <c r="D78" s="21"/>
+      <c r="E78" s="21"/>
       <c r="F78" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="G78" s="26"/>
-      <c r="H78" s="23"/>
-      <c r="I78" s="23"/>
-      <c r="J78" s="23"/>
-      <c r="K78" s="23"/>
-      <c r="L78" s="23"/>
+      <c r="G78" s="19"/>
+      <c r="H78" s="21"/>
+      <c r="I78" s="21"/>
+      <c r="J78" s="21"/>
+      <c r="K78" s="21"/>
+      <c r="L78" s="21"/>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A79" s="25"/>
-      <c r="B79" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C79" s="26"/>
-      <c r="D79" s="23"/>
-      <c r="E79" s="23" t="s">
+      <c r="A79" s="18"/>
+      <c r="B79" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C79" s="19"/>
+      <c r="D79" s="21"/>
+      <c r="E79" s="21" t="s">
         <v>248</v>
       </c>
       <c r="F79" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="G79" s="26"/>
-      <c r="H79" s="23"/>
-      <c r="I79" s="23"/>
-      <c r="J79" s="23"/>
-      <c r="K79" s="23"/>
-      <c r="L79" s="23"/>
+      <c r="G79" s="19"/>
+      <c r="H79" s="21"/>
+      <c r="I79" s="21"/>
+      <c r="J79" s="21"/>
+      <c r="K79" s="21"/>
+      <c r="L79" s="21"/>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A80" s="25" t="s">
+      <c r="A80" s="18" t="s">
         <v>236</v>
       </c>
-      <c r="B80" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C80" s="26" t="s">
+      <c r="B80" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C80" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="D80" s="23" t="s">
+      <c r="D80" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="E80" s="23" t="s">
+      <c r="E80" s="21" t="s">
         <v>248</v>
       </c>
       <c r="F80" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="G80" s="26" t="s">
+      <c r="G80" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="H80" s="23" t="s">
+      <c r="H80" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="I80" s="23" t="s">
+      <c r="I80" s="21" t="s">
         <v>305</v>
       </c>
-      <c r="J80" s="23" t="s">
+      <c r="J80" s="21" t="s">
         <v>319</v>
       </c>
-      <c r="K80" s="23"/>
-      <c r="L80" s="23"/>
+      <c r="K80" s="21"/>
+      <c r="L80" s="21"/>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A81" s="25"/>
-      <c r="B81" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C81" s="26"/>
-      <c r="D81" s="23"/>
-      <c r="E81" s="23" t="s">
+      <c r="A81" s="18"/>
+      <c r="B81" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C81" s="19"/>
+      <c r="D81" s="21"/>
+      <c r="E81" s="21" t="s">
         <v>248</v>
       </c>
       <c r="F81" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="G81" s="26"/>
-      <c r="H81" s="23"/>
-      <c r="I81" s="23"/>
-      <c r="J81" s="23"/>
-      <c r="K81" s="23"/>
-      <c r="L81" s="23"/>
+      <c r="G81" s="19"/>
+      <c r="H81" s="21"/>
+      <c r="I81" s="21"/>
+      <c r="J81" s="21"/>
+      <c r="K81" s="21"/>
+      <c r="L81" s="21"/>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A82" s="25"/>
-      <c r="B82" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C82" s="26"/>
-      <c r="D82" s="23"/>
-      <c r="E82" s="23"/>
+      <c r="A82" s="18"/>
+      <c r="B82" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C82" s="19"/>
+      <c r="D82" s="21"/>
+      <c r="E82" s="21"/>
       <c r="F82" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="G82" s="26"/>
-      <c r="H82" s="23"/>
-      <c r="I82" s="23"/>
-      <c r="J82" s="23"/>
-      <c r="K82" s="23"/>
-      <c r="L82" s="23"/>
+      <c r="G82" s="19"/>
+      <c r="H82" s="21"/>
+      <c r="I82" s="21"/>
+      <c r="J82" s="21"/>
+      <c r="K82" s="21"/>
+      <c r="L82" s="21"/>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A83" s="25"/>
-      <c r="B83" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C83" s="26"/>
-      <c r="D83" s="23"/>
-      <c r="E83" s="23" t="s">
+      <c r="A83" s="18"/>
+      <c r="B83" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C83" s="19"/>
+      <c r="D83" s="21"/>
+      <c r="E83" s="21" t="s">
         <v>248</v>
       </c>
       <c r="F83" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="G83" s="26"/>
-      <c r="H83" s="23"/>
-      <c r="I83" s="23"/>
-      <c r="J83" s="23"/>
-      <c r="K83" s="23"/>
-      <c r="L83" s="23"/>
+      <c r="G83" s="19"/>
+      <c r="H83" s="21"/>
+      <c r="I83" s="21"/>
+      <c r="J83" s="21"/>
+      <c r="K83" s="21"/>
+      <c r="L83" s="21"/>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A84" s="25"/>
-      <c r="B84" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C84" s="26"/>
-      <c r="D84" s="23"/>
-      <c r="E84" s="23"/>
+      <c r="A84" s="18"/>
+      <c r="B84" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C84" s="19"/>
+      <c r="D84" s="21"/>
+      <c r="E84" s="21"/>
       <c r="F84" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="G84" s="26"/>
-      <c r="H84" s="23"/>
-      <c r="I84" s="23"/>
-      <c r="J84" s="23"/>
-      <c r="K84" s="23"/>
-      <c r="L84" s="23"/>
+      <c r="G84" s="19"/>
+      <c r="H84" s="21"/>
+      <c r="I84" s="21"/>
+      <c r="J84" s="21"/>
+      <c r="K84" s="21"/>
+      <c r="L84" s="21"/>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A85" s="25" t="s">
+      <c r="A85" s="18" t="s">
         <v>237</v>
       </c>
-      <c r="B85" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C85" s="26" t="s">
+      <c r="B85" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C85" s="19" t="s">
         <v>144</v>
       </c>
-      <c r="D85" s="23" t="s">
+      <c r="D85" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="E85" s="23" t="s">
+      <c r="E85" s="21" t="s">
         <v>248</v>
       </c>
       <c r="F85" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="G85" s="20" t="s">
+      <c r="G85" s="29" t="s">
         <v>310</v>
       </c>
-      <c r="H85" s="18" t="s">
+      <c r="H85" s="20" t="s">
         <v>255</v>
       </c>
-      <c r="I85" s="23" t="s">
+      <c r="I85" s="21" t="s">
         <v>305</v>
       </c>
-      <c r="J85" s="23" t="s">
+      <c r="J85" s="21" t="s">
         <v>319</v>
       </c>
-      <c r="K85" s="23"/>
-      <c r="L85" s="23"/>
+      <c r="K85" s="21"/>
+      <c r="L85" s="21"/>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A86" s="25"/>
-      <c r="B86" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C86" s="26"/>
-      <c r="D86" s="23"/>
-      <c r="E86" s="23" t="s">
+      <c r="A86" s="18"/>
+      <c r="B86" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C86" s="19"/>
+      <c r="D86" s="21"/>
+      <c r="E86" s="21" t="s">
         <v>248</v>
       </c>
       <c r="F86" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="G86" s="26"/>
-      <c r="H86" s="23"/>
-      <c r="I86" s="23"/>
-      <c r="J86" s="23"/>
-      <c r="K86" s="23"/>
-      <c r="L86" s="23"/>
+      <c r="G86" s="19"/>
+      <c r="H86" s="21"/>
+      <c r="I86" s="21"/>
+      <c r="J86" s="21"/>
+      <c r="K86" s="21"/>
+      <c r="L86" s="21"/>
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A87" s="25"/>
-      <c r="B87" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C87" s="26"/>
-      <c r="D87" s="23"/>
-      <c r="E87" s="23"/>
+      <c r="A87" s="18"/>
+      <c r="B87" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C87" s="19"/>
+      <c r="D87" s="21"/>
+      <c r="E87" s="21"/>
       <c r="F87" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="G87" s="26"/>
-      <c r="H87" s="23"/>
-      <c r="I87" s="23"/>
-      <c r="J87" s="23"/>
-      <c r="K87" s="23"/>
-      <c r="L87" s="23"/>
+      <c r="G87" s="19"/>
+      <c r="H87" s="21"/>
+      <c r="I87" s="21"/>
+      <c r="J87" s="21"/>
+      <c r="K87" s="21"/>
+      <c r="L87" s="21"/>
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A88" s="25"/>
-      <c r="B88" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C88" s="26"/>
-      <c r="D88" s="23"/>
-      <c r="E88" s="23" t="s">
+      <c r="A88" s="18"/>
+      <c r="B88" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C88" s="19"/>
+      <c r="D88" s="21"/>
+      <c r="E88" s="21" t="s">
         <v>248</v>
       </c>
       <c r="F88" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="G88" s="26"/>
-      <c r="H88" s="23"/>
-      <c r="I88" s="23"/>
-      <c r="J88" s="23"/>
-      <c r="K88" s="23"/>
-      <c r="L88" s="23"/>
+      <c r="G88" s="19"/>
+      <c r="H88" s="21"/>
+      <c r="I88" s="21"/>
+      <c r="J88" s="21"/>
+      <c r="K88" s="21"/>
+      <c r="L88" s="21"/>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A89" s="25"/>
-      <c r="B89" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C89" s="26"/>
-      <c r="D89" s="23"/>
-      <c r="E89" s="23"/>
+      <c r="A89" s="18"/>
+      <c r="B89" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C89" s="19"/>
+      <c r="D89" s="21"/>
+      <c r="E89" s="21"/>
       <c r="F89" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="G89" s="26"/>
-      <c r="H89" s="23"/>
-      <c r="I89" s="23"/>
-      <c r="J89" s="23"/>
-      <c r="K89" s="23"/>
-      <c r="L89" s="23"/>
+      <c r="G89" s="19"/>
+      <c r="H89" s="21"/>
+      <c r="I89" s="21"/>
+      <c r="J89" s="21"/>
+      <c r="K89" s="21"/>
+      <c r="L89" s="21"/>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A90" s="25" t="s">
+      <c r="A90" s="18" t="s">
         <v>238</v>
       </c>
-      <c r="B90" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C90" s="26" t="s">
+      <c r="B90" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C90" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="D90" s="23" t="s">
+      <c r="D90" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="E90" s="23" t="s">
+      <c r="E90" s="21" t="s">
         <v>248</v>
       </c>
       <c r="F90" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="G90" s="20" t="s">
+      <c r="G90" s="29" t="s">
         <v>318</v>
       </c>
-      <c r="H90" s="18" t="s">
+      <c r="H90" s="20" t="s">
         <v>256</v>
       </c>
-      <c r="I90" s="23" t="s">
+      <c r="I90" s="21" t="s">
         <v>305</v>
       </c>
-      <c r="J90" s="23" t="s">
+      <c r="J90" s="21" t="s">
         <v>319</v>
       </c>
-      <c r="K90" s="23"/>
-      <c r="L90" s="23"/>
+      <c r="K90" s="21"/>
+      <c r="L90" s="21"/>
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A91" s="25"/>
-      <c r="B91" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C91" s="26"/>
-      <c r="D91" s="23"/>
-      <c r="E91" s="23"/>
+      <c r="A91" s="18"/>
+      <c r="B91" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C91" s="19"/>
+      <c r="D91" s="21"/>
+      <c r="E91" s="21"/>
       <c r="F91" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="G91" s="20"/>
-      <c r="H91" s="18"/>
-      <c r="I91" s="23"/>
-      <c r="J91" s="23"/>
-      <c r="K91" s="23"/>
-      <c r="L91" s="23"/>
+      <c r="G91" s="29"/>
+      <c r="H91" s="20"/>
+      <c r="I91" s="21"/>
+      <c r="J91" s="21"/>
+      <c r="K91" s="21"/>
+      <c r="L91" s="21"/>
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A92" s="25"/>
-      <c r="B92" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C92" s="26"/>
-      <c r="D92" s="23"/>
-      <c r="E92" s="23" t="s">
+      <c r="A92" s="18"/>
+      <c r="B92" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C92" s="19"/>
+      <c r="D92" s="21"/>
+      <c r="E92" s="21" t="s">
         <v>248</v>
       </c>
       <c r="F92" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="G92" s="20"/>
-      <c r="H92" s="18"/>
-      <c r="I92" s="23"/>
-      <c r="J92" s="23"/>
-      <c r="K92" s="23"/>
-      <c r="L92" s="23"/>
+      <c r="G92" s="29"/>
+      <c r="H92" s="20"/>
+      <c r="I92" s="21"/>
+      <c r="J92" s="21"/>
+      <c r="K92" s="21"/>
+      <c r="L92" s="21"/>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A93" s="25"/>
-      <c r="B93" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C93" s="26"/>
-      <c r="D93" s="23"/>
-      <c r="E93" s="23"/>
+      <c r="A93" s="18"/>
+      <c r="B93" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C93" s="19"/>
+      <c r="D93" s="21"/>
+      <c r="E93" s="21"/>
       <c r="F93" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="G93" s="20"/>
-      <c r="H93" s="18"/>
-      <c r="I93" s="23"/>
-      <c r="J93" s="23"/>
-      <c r="K93" s="23"/>
-      <c r="L93" s="23"/>
+      <c r="G93" s="29"/>
+      <c r="H93" s="20"/>
+      <c r="I93" s="21"/>
+      <c r="J93" s="21"/>
+      <c r="K93" s="21"/>
+      <c r="L93" s="21"/>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A94" s="25" t="s">
+      <c r="A94" s="18" t="s">
         <v>239</v>
       </c>
-      <c r="B94" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C94" s="26" t="s">
+      <c r="B94" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C94" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="D94" s="23" t="s">
+      <c r="D94" s="21" t="s">
         <v>133</v>
       </c>
-      <c r="E94" s="23" t="s">
+      <c r="E94" s="21" t="s">
         <v>248</v>
       </c>
       <c r="F94" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="G94" s="26" t="s">
+      <c r="G94" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="H94" s="23" t="s">
+      <c r="H94" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="I94" s="23"/>
-      <c r="J94" s="26" t="s">
+      <c r="I94" s="19" t="s">
+        <v>305</v>
+      </c>
+      <c r="J94" s="19" t="s">
         <v>319</v>
       </c>
-      <c r="K94" s="23"/>
-      <c r="L94" s="23"/>
+      <c r="K94" s="21"/>
+      <c r="L94" s="21"/>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A95" s="25"/>
-      <c r="B95" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C95" s="26"/>
-      <c r="D95" s="23"/>
-      <c r="E95" s="23" t="s">
+      <c r="A95" s="18"/>
+      <c r="B95" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C95" s="19"/>
+      <c r="D95" s="21"/>
+      <c r="E95" s="21" t="s">
         <v>248</v>
       </c>
       <c r="F95" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="G95" s="26"/>
-      <c r="H95" s="23"/>
-      <c r="I95" s="23"/>
-      <c r="J95" s="26"/>
-      <c r="K95" s="23"/>
-      <c r="L95" s="23"/>
+      <c r="G95" s="19"/>
+      <c r="H95" s="21"/>
+      <c r="I95" s="19"/>
+      <c r="J95" s="19"/>
+      <c r="K95" s="21"/>
+      <c r="L95" s="21"/>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A96" s="25"/>
-      <c r="B96" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C96" s="26"/>
-      <c r="D96" s="23"/>
-      <c r="E96" s="23"/>
+      <c r="A96" s="18"/>
+      <c r="B96" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C96" s="19"/>
+      <c r="D96" s="21"/>
+      <c r="E96" s="21"/>
       <c r="F96" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="G96" s="26"/>
-      <c r="H96" s="23"/>
-      <c r="I96" s="23"/>
-      <c r="J96" s="26"/>
-      <c r="K96" s="23"/>
-      <c r="L96" s="23"/>
+      <c r="G96" s="19"/>
+      <c r="H96" s="21"/>
+      <c r="I96" s="19"/>
+      <c r="J96" s="19"/>
+      <c r="K96" s="21"/>
+      <c r="L96" s="21"/>
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A97" s="25"/>
-      <c r="B97" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C97" s="26"/>
-      <c r="D97" s="23"/>
-      <c r="E97" s="23" t="s">
+      <c r="A97" s="18"/>
+      <c r="B97" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C97" s="19"/>
+      <c r="D97" s="21"/>
+      <c r="E97" s="21" t="s">
         <v>248</v>
       </c>
       <c r="F97" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="G97" s="26"/>
-      <c r="H97" s="23"/>
-      <c r="I97" s="23"/>
-      <c r="J97" s="26"/>
-      <c r="K97" s="23"/>
-      <c r="L97" s="23"/>
+      <c r="G97" s="19"/>
+      <c r="H97" s="21"/>
+      <c r="I97" s="19"/>
+      <c r="J97" s="19"/>
+      <c r="K97" s="21"/>
+      <c r="L97" s="21"/>
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A98" s="25"/>
-      <c r="B98" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C98" s="26"/>
-      <c r="D98" s="23"/>
-      <c r="E98" s="23"/>
+      <c r="A98" s="18"/>
+      <c r="B98" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C98" s="19"/>
+      <c r="D98" s="21"/>
+      <c r="E98" s="21"/>
       <c r="F98" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="G98" s="26"/>
-      <c r="H98" s="23"/>
-      <c r="I98" s="23"/>
-      <c r="J98" s="26"/>
-      <c r="K98" s="23"/>
-      <c r="L98" s="23"/>
+      <c r="G98" s="19"/>
+      <c r="H98" s="21"/>
+      <c r="I98" s="19"/>
+      <c r="J98" s="19"/>
+      <c r="K98" s="21"/>
+      <c r="L98" s="21"/>
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A99" s="25" t="s">
+      <c r="A99" s="18" t="s">
         <v>240</v>
       </c>
-      <c r="B99" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C99" s="26" t="s">
+      <c r="B99" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C99" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="D99" s="23" t="s">
+      <c r="D99" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="E99" s="23" t="s">
+      <c r="E99" s="21" t="s">
         <v>248</v>
       </c>
       <c r="F99" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="G99" s="26" t="s">
+      <c r="G99" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="H99" s="23" t="s">
+      <c r="H99" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="I99" s="19"/>
-      <c r="J99" s="20" t="s">
+      <c r="I99" s="29" t="s">
+        <v>305</v>
+      </c>
+      <c r="J99" s="29" t="s">
         <v>319</v>
       </c>
-      <c r="K99" s="19"/>
-      <c r="L99" s="19"/>
+      <c r="K99" s="28"/>
+      <c r="L99" s="28"/>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A100" s="25"/>
-      <c r="B100" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C100" s="26"/>
-      <c r="D100" s="23"/>
-      <c r="E100" s="23"/>
+      <c r="A100" s="18"/>
+      <c r="B100" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C100" s="19"/>
+      <c r="D100" s="21"/>
+      <c r="E100" s="21"/>
       <c r="F100" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="G100" s="26"/>
-      <c r="H100" s="23"/>
-      <c r="I100" s="19"/>
-      <c r="J100" s="20"/>
-      <c r="K100" s="19"/>
-      <c r="L100" s="19"/>
+      <c r="G100" s="19"/>
+      <c r="H100" s="21"/>
+      <c r="I100" s="29"/>
+      <c r="J100" s="29"/>
+      <c r="K100" s="28"/>
+      <c r="L100" s="28"/>
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A101" s="25"/>
-      <c r="B101" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C101" s="26"/>
-      <c r="D101" s="23"/>
-      <c r="E101" s="23" t="s">
+      <c r="A101" s="18"/>
+      <c r="B101" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C101" s="19"/>
+      <c r="D101" s="21"/>
+      <c r="E101" s="21" t="s">
         <v>248</v>
       </c>
       <c r="F101" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="G101" s="26"/>
-      <c r="H101" s="23"/>
-      <c r="I101" s="19"/>
-      <c r="J101" s="20"/>
-      <c r="K101" s="19"/>
-      <c r="L101" s="19"/>
+      <c r="G101" s="19"/>
+      <c r="H101" s="21"/>
+      <c r="I101" s="29"/>
+      <c r="J101" s="29"/>
+      <c r="K101" s="28"/>
+      <c r="L101" s="28"/>
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A102" s="25"/>
-      <c r="B102" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C102" s="26"/>
-      <c r="D102" s="23"/>
-      <c r="E102" s="23"/>
+      <c r="A102" s="18"/>
+      <c r="B102" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C102" s="19"/>
+      <c r="D102" s="21"/>
+      <c r="E102" s="21"/>
       <c r="F102" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="G102" s="26"/>
-      <c r="H102" s="23"/>
-      <c r="I102" s="19"/>
-      <c r="J102" s="20"/>
-      <c r="K102" s="19"/>
-      <c r="L102" s="19"/>
+      <c r="G102" s="19"/>
+      <c r="H102" s="21"/>
+      <c r="I102" s="29"/>
+      <c r="J102" s="29"/>
+      <c r="K102" s="28"/>
+      <c r="L102" s="28"/>
     </row>
     <row r="129" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H129" s="14"/>
@@ -4025,61 +4026,205 @@
     </row>
   </sheetData>
   <mergeCells count="297">
-    <mergeCell ref="A23:A28"/>
-    <mergeCell ref="C23:C28"/>
-    <mergeCell ref="H23:H28"/>
-    <mergeCell ref="I23:I28"/>
-    <mergeCell ref="J23:J28"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="C29:C32"/>
-    <mergeCell ref="H29:H32"/>
-    <mergeCell ref="I29:I32"/>
-    <mergeCell ref="J29:J32"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="C33:C35"/>
-    <mergeCell ref="H33:H35"/>
-    <mergeCell ref="I33:I35"/>
-    <mergeCell ref="J33:J35"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="C36:C39"/>
-    <mergeCell ref="H36:H39"/>
-    <mergeCell ref="I36:I39"/>
-    <mergeCell ref="J36:J39"/>
-    <mergeCell ref="A58:A61"/>
-    <mergeCell ref="C58:C61"/>
-    <mergeCell ref="H58:H61"/>
-    <mergeCell ref="I58:I61"/>
-    <mergeCell ref="J58:J61"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="C40:C43"/>
-    <mergeCell ref="H40:H43"/>
-    <mergeCell ref="I40:I43"/>
-    <mergeCell ref="J40:J43"/>
-    <mergeCell ref="A75:A79"/>
-    <mergeCell ref="C75:C79"/>
-    <mergeCell ref="H75:H79"/>
-    <mergeCell ref="I75:I79"/>
-    <mergeCell ref="J75:J79"/>
-    <mergeCell ref="A62:A65"/>
-    <mergeCell ref="C62:C65"/>
-    <mergeCell ref="H62:H65"/>
-    <mergeCell ref="I62:I65"/>
-    <mergeCell ref="J62:J65"/>
-    <mergeCell ref="A66:A69"/>
-    <mergeCell ref="C66:C69"/>
-    <mergeCell ref="H66:H69"/>
-    <mergeCell ref="I66:I69"/>
-    <mergeCell ref="J66:J69"/>
-    <mergeCell ref="A99:A102"/>
-    <mergeCell ref="C99:C102"/>
-    <mergeCell ref="H99:H102"/>
-    <mergeCell ref="I99:I102"/>
-    <mergeCell ref="J99:J102"/>
-    <mergeCell ref="A90:A93"/>
-    <mergeCell ref="C90:C93"/>
-    <mergeCell ref="H90:H93"/>
-    <mergeCell ref="I90:I93"/>
-    <mergeCell ref="J90:J93"/>
+    <mergeCell ref="G51:G54"/>
+    <mergeCell ref="G55:G57"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="G23:G28"/>
+    <mergeCell ref="G29:G32"/>
+    <mergeCell ref="G33:G35"/>
+    <mergeCell ref="G94:G98"/>
+    <mergeCell ref="G80:G84"/>
+    <mergeCell ref="G85:G89"/>
+    <mergeCell ref="G90:G93"/>
+    <mergeCell ref="G58:G61"/>
+    <mergeCell ref="G62:G65"/>
+    <mergeCell ref="G66:G69"/>
+    <mergeCell ref="G70:G74"/>
+    <mergeCell ref="G75:G79"/>
+    <mergeCell ref="A47:A50"/>
+    <mergeCell ref="E47:E50"/>
+    <mergeCell ref="I47:I50"/>
+    <mergeCell ref="I51:I54"/>
+    <mergeCell ref="I55:I57"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="B51:B54"/>
+    <mergeCell ref="B55:B57"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="E23:E28"/>
+    <mergeCell ref="E29:E32"/>
+    <mergeCell ref="E33:E35"/>
+    <mergeCell ref="E36:E39"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="L51:L54"/>
+    <mergeCell ref="L55:L57"/>
+    <mergeCell ref="L44:L46"/>
+    <mergeCell ref="L47:L50"/>
+    <mergeCell ref="L94:L98"/>
+    <mergeCell ref="L99:L102"/>
+    <mergeCell ref="L80:L84"/>
+    <mergeCell ref="L85:L89"/>
+    <mergeCell ref="L90:L93"/>
+    <mergeCell ref="L58:L61"/>
+    <mergeCell ref="L62:L65"/>
+    <mergeCell ref="L66:L69"/>
+    <mergeCell ref="L70:L74"/>
+    <mergeCell ref="L75:L79"/>
+    <mergeCell ref="L23:L28"/>
+    <mergeCell ref="L29:L32"/>
+    <mergeCell ref="L33:L35"/>
+    <mergeCell ref="L36:L39"/>
+    <mergeCell ref="L40:L43"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="L12:L13"/>
+    <mergeCell ref="L15:L16"/>
+    <mergeCell ref="L17:L18"/>
+    <mergeCell ref="L19:L20"/>
+    <mergeCell ref="L21:L22"/>
+    <mergeCell ref="B85:B89"/>
+    <mergeCell ref="B90:B93"/>
+    <mergeCell ref="B94:B98"/>
+    <mergeCell ref="B99:B102"/>
+    <mergeCell ref="B66:B69"/>
+    <mergeCell ref="B70:B74"/>
+    <mergeCell ref="B75:B79"/>
+    <mergeCell ref="B80:B84"/>
+    <mergeCell ref="E90:E93"/>
+    <mergeCell ref="E94:E98"/>
+    <mergeCell ref="E99:E102"/>
+    <mergeCell ref="E70:E74"/>
+    <mergeCell ref="E75:E79"/>
+    <mergeCell ref="E80:E84"/>
+    <mergeCell ref="E85:E89"/>
+    <mergeCell ref="E66:E69"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="B58:B61"/>
+    <mergeCell ref="B62:B65"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B23:B28"/>
+    <mergeCell ref="B29:B32"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="E40:E43"/>
+    <mergeCell ref="E58:E61"/>
+    <mergeCell ref="E62:E65"/>
+    <mergeCell ref="E51:E54"/>
+    <mergeCell ref="E55:E57"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="E44:E46"/>
+    <mergeCell ref="B47:B50"/>
+    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="B40:B43"/>
+    <mergeCell ref="G36:G39"/>
+    <mergeCell ref="G40:G43"/>
+    <mergeCell ref="G44:G46"/>
+    <mergeCell ref="G47:G50"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="K17:K18"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="K19:K20"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="K12:K13"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="K15:K16"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="K21:K22"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="D80:D84"/>
+    <mergeCell ref="D85:D89"/>
+    <mergeCell ref="D90:D93"/>
+    <mergeCell ref="D58:D61"/>
+    <mergeCell ref="D62:D65"/>
+    <mergeCell ref="D66:D69"/>
+    <mergeCell ref="D70:D74"/>
+    <mergeCell ref="D75:D79"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="K44:K46"/>
+    <mergeCell ref="I44:I46"/>
+    <mergeCell ref="K94:K98"/>
+    <mergeCell ref="K99:K102"/>
+    <mergeCell ref="D94:D98"/>
+    <mergeCell ref="D99:D102"/>
+    <mergeCell ref="K80:K84"/>
+    <mergeCell ref="K85:K89"/>
+    <mergeCell ref="K90:K93"/>
+    <mergeCell ref="K58:K61"/>
+    <mergeCell ref="K62:K65"/>
+    <mergeCell ref="K66:K69"/>
+    <mergeCell ref="K70:K74"/>
+    <mergeCell ref="K75:K79"/>
+    <mergeCell ref="J70:J74"/>
+    <mergeCell ref="K55:K57"/>
+    <mergeCell ref="D51:D54"/>
+    <mergeCell ref="H51:H54"/>
+    <mergeCell ref="J51:J54"/>
+    <mergeCell ref="K51:K54"/>
+    <mergeCell ref="D47:D50"/>
+    <mergeCell ref="H47:H50"/>
+    <mergeCell ref="J47:J50"/>
+    <mergeCell ref="K47:K50"/>
     <mergeCell ref="K23:K28"/>
     <mergeCell ref="K29:K32"/>
     <mergeCell ref="K33:K35"/>
@@ -4104,36 +4249,44 @@
     <mergeCell ref="C70:C74"/>
     <mergeCell ref="H70:H74"/>
     <mergeCell ref="I70:I74"/>
-    <mergeCell ref="K44:K46"/>
-    <mergeCell ref="I44:I46"/>
-    <mergeCell ref="K94:K98"/>
-    <mergeCell ref="K99:K102"/>
-    <mergeCell ref="D94:D98"/>
-    <mergeCell ref="D99:D102"/>
-    <mergeCell ref="K80:K84"/>
-    <mergeCell ref="K85:K89"/>
-    <mergeCell ref="K90:K93"/>
-    <mergeCell ref="K58:K61"/>
-    <mergeCell ref="K62:K65"/>
-    <mergeCell ref="K66:K69"/>
-    <mergeCell ref="K70:K74"/>
-    <mergeCell ref="K75:K79"/>
-    <mergeCell ref="J70:J74"/>
-    <mergeCell ref="K55:K57"/>
+    <mergeCell ref="A99:A102"/>
+    <mergeCell ref="C99:C102"/>
+    <mergeCell ref="H99:H102"/>
+    <mergeCell ref="I99:I102"/>
+    <mergeCell ref="J99:J102"/>
+    <mergeCell ref="A90:A93"/>
+    <mergeCell ref="C90:C93"/>
+    <mergeCell ref="H90:H93"/>
+    <mergeCell ref="I90:I93"/>
+    <mergeCell ref="J90:J93"/>
+    <mergeCell ref="G99:G102"/>
+    <mergeCell ref="A75:A79"/>
+    <mergeCell ref="C75:C79"/>
+    <mergeCell ref="H75:H79"/>
+    <mergeCell ref="I75:I79"/>
+    <mergeCell ref="J75:J79"/>
+    <mergeCell ref="A62:A65"/>
+    <mergeCell ref="C62:C65"/>
+    <mergeCell ref="H62:H65"/>
+    <mergeCell ref="I62:I65"/>
+    <mergeCell ref="J62:J65"/>
+    <mergeCell ref="A66:A69"/>
+    <mergeCell ref="C66:C69"/>
+    <mergeCell ref="H66:H69"/>
+    <mergeCell ref="I66:I69"/>
+    <mergeCell ref="J66:J69"/>
+    <mergeCell ref="A58:A61"/>
+    <mergeCell ref="C58:C61"/>
+    <mergeCell ref="H58:H61"/>
+    <mergeCell ref="I58:I61"/>
+    <mergeCell ref="J58:J61"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="C40:C43"/>
+    <mergeCell ref="H40:H43"/>
+    <mergeCell ref="I40:I43"/>
+    <mergeCell ref="J40:J43"/>
     <mergeCell ref="C51:C54"/>
-    <mergeCell ref="D51:D54"/>
-    <mergeCell ref="H51:H54"/>
-    <mergeCell ref="J51:J54"/>
-    <mergeCell ref="K51:K54"/>
     <mergeCell ref="C47:C50"/>
-    <mergeCell ref="D47:D50"/>
-    <mergeCell ref="H47:H50"/>
-    <mergeCell ref="J47:J50"/>
-    <mergeCell ref="K47:K50"/>
-    <mergeCell ref="D23:D28"/>
-    <mergeCell ref="D29:D32"/>
-    <mergeCell ref="D33:D35"/>
-    <mergeCell ref="D36:D39"/>
     <mergeCell ref="D40:D43"/>
     <mergeCell ref="C55:C57"/>
     <mergeCell ref="D55:D57"/>
@@ -4143,185 +4296,33 @@
     <mergeCell ref="D44:D46"/>
     <mergeCell ref="H44:H46"/>
     <mergeCell ref="J44:J46"/>
-    <mergeCell ref="D80:D84"/>
-    <mergeCell ref="D85:D89"/>
-    <mergeCell ref="D90:D93"/>
-    <mergeCell ref="D58:D61"/>
-    <mergeCell ref="D62:D65"/>
-    <mergeCell ref="D66:D69"/>
-    <mergeCell ref="D70:D74"/>
-    <mergeCell ref="D75:D79"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="H21:H22"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="J4:J5"/>
-    <mergeCell ref="K4:K5"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="I21:I22"/>
-    <mergeCell ref="J21:J22"/>
-    <mergeCell ref="K21:K22"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="K17:K18"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="K19:K20"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="K12:K13"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="K15:K16"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="B58:B61"/>
-    <mergeCell ref="B62:B65"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B23:B28"/>
-    <mergeCell ref="B29:B32"/>
-    <mergeCell ref="B33:B35"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B85:B89"/>
-    <mergeCell ref="B90:B93"/>
-    <mergeCell ref="B94:B98"/>
-    <mergeCell ref="B99:B102"/>
-    <mergeCell ref="B66:B69"/>
-    <mergeCell ref="B70:B74"/>
-    <mergeCell ref="B75:B79"/>
-    <mergeCell ref="B80:B84"/>
-    <mergeCell ref="E90:E93"/>
-    <mergeCell ref="E94:E98"/>
-    <mergeCell ref="E99:E102"/>
-    <mergeCell ref="E70:E74"/>
-    <mergeCell ref="E75:E79"/>
-    <mergeCell ref="E80:E84"/>
-    <mergeCell ref="E85:E89"/>
-    <mergeCell ref="E40:E43"/>
-    <mergeCell ref="E58:E61"/>
-    <mergeCell ref="E62:E65"/>
-    <mergeCell ref="E66:E69"/>
-    <mergeCell ref="L23:L28"/>
-    <mergeCell ref="L29:L32"/>
-    <mergeCell ref="L33:L35"/>
-    <mergeCell ref="L36:L39"/>
-    <mergeCell ref="L40:L43"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="L4:L5"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="L12:L13"/>
-    <mergeCell ref="L15:L16"/>
-    <mergeCell ref="L17:L18"/>
-    <mergeCell ref="L19:L20"/>
-    <mergeCell ref="L21:L22"/>
-    <mergeCell ref="L51:L54"/>
-    <mergeCell ref="L55:L57"/>
-    <mergeCell ref="L44:L46"/>
-    <mergeCell ref="L47:L50"/>
-    <mergeCell ref="L94:L98"/>
-    <mergeCell ref="L99:L102"/>
-    <mergeCell ref="L80:L84"/>
-    <mergeCell ref="L85:L89"/>
-    <mergeCell ref="L90:L93"/>
-    <mergeCell ref="L58:L61"/>
-    <mergeCell ref="L62:L65"/>
-    <mergeCell ref="L66:L69"/>
-    <mergeCell ref="L70:L74"/>
-    <mergeCell ref="L75:L79"/>
     <mergeCell ref="A51:A54"/>
     <mergeCell ref="A55:A57"/>
-    <mergeCell ref="E51:E54"/>
-    <mergeCell ref="E55:E57"/>
-    <mergeCell ref="B44:B46"/>
     <mergeCell ref="A44:A46"/>
-    <mergeCell ref="E44:E46"/>
-    <mergeCell ref="B47:B50"/>
-    <mergeCell ref="A47:A50"/>
-    <mergeCell ref="E47:E50"/>
-    <mergeCell ref="I47:I50"/>
-    <mergeCell ref="I51:I54"/>
-    <mergeCell ref="I55:I57"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="B51:B54"/>
-    <mergeCell ref="B55:B57"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="E23:E28"/>
-    <mergeCell ref="E29:E32"/>
-    <mergeCell ref="E33:E35"/>
-    <mergeCell ref="E36:E39"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="B36:B39"/>
-    <mergeCell ref="B40:B43"/>
-    <mergeCell ref="G36:G39"/>
-    <mergeCell ref="G40:G43"/>
-    <mergeCell ref="G44:G46"/>
-    <mergeCell ref="G47:G50"/>
-    <mergeCell ref="G51:G54"/>
-    <mergeCell ref="G55:G57"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="G23:G28"/>
-    <mergeCell ref="G29:G32"/>
-    <mergeCell ref="G33:G35"/>
-    <mergeCell ref="G94:G98"/>
-    <mergeCell ref="G99:G102"/>
-    <mergeCell ref="G80:G84"/>
-    <mergeCell ref="G85:G89"/>
-    <mergeCell ref="G90:G93"/>
-    <mergeCell ref="G58:G61"/>
-    <mergeCell ref="G62:G65"/>
-    <mergeCell ref="G66:G69"/>
-    <mergeCell ref="G70:G74"/>
-    <mergeCell ref="G75:G79"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="C33:C35"/>
+    <mergeCell ref="H33:H35"/>
+    <mergeCell ref="I33:I35"/>
+    <mergeCell ref="J33:J35"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="C36:C39"/>
+    <mergeCell ref="H36:H39"/>
+    <mergeCell ref="I36:I39"/>
+    <mergeCell ref="J36:J39"/>
+    <mergeCell ref="D33:D35"/>
+    <mergeCell ref="D36:D39"/>
+    <mergeCell ref="A23:A28"/>
+    <mergeCell ref="C23:C28"/>
+    <mergeCell ref="H23:H28"/>
+    <mergeCell ref="I23:I28"/>
+    <mergeCell ref="J23:J28"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="C29:C32"/>
+    <mergeCell ref="H29:H32"/>
+    <mergeCell ref="I29:I32"/>
+    <mergeCell ref="J29:J32"/>
+    <mergeCell ref="D23:D28"/>
+    <mergeCell ref="D29:D32"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4754,56 +4755,56 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="31" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="31" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="27"/>
-      <c r="B3" s="27"/>
+      <c r="A3" s="31"/>
+      <c r="B3" s="31"/>
       <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="27"/>
+      <c r="D3" s="31"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="31" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="31" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="27"/>
-      <c r="B5" s="27"/>
+      <c r="A5" s="31"/>
+      <c r="B5" s="31"/>
       <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="27"/>
+      <c r="D5" s="31"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="27"/>
-      <c r="B6" s="27"/>
+      <c r="A6" s="31"/>
+      <c r="B6" s="31"/>
       <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="27"/>
+      <c r="D6" s="31"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
@@ -4848,48 +4849,48 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="31" t="s">
         <v>28</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="27" t="s">
+      <c r="D10" s="31" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="27"/>
-      <c r="B11" s="27"/>
+      <c r="A11" s="31"/>
+      <c r="B11" s="31"/>
       <c r="C11" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="27"/>
+      <c r="D11" s="31"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="31" t="s">
         <v>33</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="27" t="s">
+      <c r="D12" s="31" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="27"/>
-      <c r="B13" s="27"/>
+      <c r="A13" s="31"/>
+      <c r="B13" s="31"/>
       <c r="C13" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="27"/>
+      <c r="D13" s="31"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
@@ -4934,137 +4935,131 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="27" t="s">
+      <c r="A17" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="27" t="s">
+      <c r="B17" s="31" t="s">
         <v>50</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D17" s="27" t="s">
+      <c r="D17" s="31" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="27"/>
-      <c r="B18" s="27"/>
+      <c r="A18" s="31"/>
+      <c r="B18" s="31"/>
       <c r="C18" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D18" s="27"/>
+      <c r="D18" s="31"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="27" t="s">
+      <c r="A19" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="27" t="s">
+      <c r="B19" s="31" t="s">
         <v>56</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D19" s="27" t="s">
+      <c r="D19" s="31" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="27"/>
-      <c r="B20" s="27"/>
+      <c r="A20" s="31"/>
+      <c r="B20" s="31"/>
       <c r="C20" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D20" s="27"/>
+      <c r="D20" s="31"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="27" t="s">
+      <c r="A21" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="B21" s="27" t="s">
+      <c r="B21" s="31" t="s">
         <v>61</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D21" s="27" t="s">
+      <c r="D21" s="31" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="27"/>
-      <c r="B22" s="27"/>
+      <c r="A22" s="31"/>
+      <c r="B22" s="31"/>
       <c r="C22" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D22" s="27"/>
+      <c r="D22" s="31"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="27" t="s">
+      <c r="A23" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="B23" s="27" t="s">
+      <c r="B23" s="31" t="s">
         <v>64</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D23" s="27" t="s">
+      <c r="D23" s="31" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="27"/>
-      <c r="B24" s="27"/>
+      <c r="A24" s="31"/>
+      <c r="B24" s="31"/>
       <c r="C24" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D24" s="27"/>
+      <c r="D24" s="31"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="27" t="s">
+      <c r="A25" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="B25" s="27" t="s">
+      <c r="B25" s="31" t="s">
         <v>68</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D25" s="27" t="s">
+      <c r="D25" s="31" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="27"/>
-      <c r="B26" s="27"/>
+      <c r="A26" s="31"/>
+      <c r="B26" s="31"/>
       <c r="C26" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D26" s="27"/>
+      <c r="D26" s="31"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="27"/>
-      <c r="B27" s="27"/>
+      <c r="A27" s="31"/>
+      <c r="B27" s="31"/>
       <c r="C27" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D27" s="27"/>
+      <c r="D27" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="D25:D27"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="D21:D22"/>
@@ -5074,12 +5069,18 @@
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="D19:D20"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="B25:B27"/>
-    <mergeCell ref="D25:D27"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="D4:D6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
assesment testcases for compose gmail functionality
</commit_message>
<xml_diff>
--- a/Assessment_Testcases.xlsx
+++ b/Assessment_Testcases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MyLocal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43F781E2-32A4-4FC5-980D-21789D31477B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED0F50B-DF5E-4D1E-B789-31C30DFC537E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8F82FB5E-0F38-4637-B99A-510675DA02B5}"/>
   </bookViews>
@@ -1194,10 +1194,10 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1600,9 +1600,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCDC6287-C9DF-48D0-A699-A65D1ACAEAC9}">
   <dimension ref="A1:L139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H110" sqref="H110"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H90" sqref="H90:H93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1661,104 +1661,104 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="29" t="s">
         <v>79</v>
       </c>
       <c r="B2" s="20" t="s">
         <v>246</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="28" t="s">
         <v>142</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="28" t="s">
         <v>192</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="28" t="s">
         <v>248</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="G2" s="29" t="s">
+      <c r="G2" s="28" t="s">
         <v>310</v>
       </c>
-      <c r="H2" s="29" t="s">
+      <c r="H2" s="28" t="s">
         <v>222</v>
       </c>
-      <c r="I2" s="29" t="s">
+      <c r="I2" s="28" t="s">
         <v>305</v>
       </c>
-      <c r="J2" s="29" t="s">
+      <c r="J2" s="28" t="s">
         <v>319</v>
       </c>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="28"/>
+      <c r="A3" s="29"/>
       <c r="B3" s="20"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
       <c r="F3" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="29" t="s">
         <v>87</v>
       </c>
       <c r="B4" s="20" t="s">
         <v>246</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="28" t="s">
         <v>142</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="D4" s="28" t="s">
         <v>193</v>
       </c>
-      <c r="E4" s="29" t="s">
+      <c r="E4" s="28" t="s">
         <v>248</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="G4" s="29" t="s">
+      <c r="G4" s="28" t="s">
         <v>310</v>
       </c>
-      <c r="H4" s="29" t="s">
+      <c r="H4" s="28" t="s">
         <v>223</v>
       </c>
-      <c r="I4" s="29" t="s">
+      <c r="I4" s="28" t="s">
         <v>305</v>
       </c>
-      <c r="J4" s="29" t="s">
+      <c r="J4" s="28" t="s">
         <v>319</v>
       </c>
-      <c r="K4" s="29"/>
-      <c r="L4" s="29"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="28"/>
+      <c r="A5" s="29"/>
       <c r="B5" s="20"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
       <c r="F5" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="29"/>
-      <c r="J5" s="29"/>
-      <c r="K5" s="29"/>
-      <c r="L5" s="29"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="28"/>
+      <c r="L5" s="28"/>
     </row>
     <row r="6" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
@@ -1863,58 +1863,58 @@
       <c r="L8" s="8"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="29" t="s">
         <v>92</v>
       </c>
       <c r="B9" s="20" t="s">
         <v>246</v>
       </c>
-      <c r="C9" s="29" t="s">
+      <c r="C9" s="28" t="s">
         <v>143</v>
       </c>
-      <c r="D9" s="29" t="s">
+      <c r="D9" s="28" t="s">
         <v>197</v>
       </c>
-      <c r="E9" s="29" t="s">
+      <c r="E9" s="28" t="s">
         <v>248</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>213</v>
       </c>
-      <c r="G9" s="29" t="s">
+      <c r="G9" s="28" t="s">
         <v>310</v>
       </c>
-      <c r="H9" s="29" t="s">
+      <c r="H9" s="28" t="s">
         <v>244</v>
       </c>
-      <c r="I9" s="29" t="s">
+      <c r="I9" s="28" t="s">
         <v>305</v>
       </c>
-      <c r="J9" s="29" t="s">
+      <c r="J9" s="28" t="s">
         <v>319</v>
       </c>
-      <c r="K9" s="29"/>
-      <c r="L9" s="29"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="28"/>
+      <c r="A10" s="29"/>
       <c r="B10" s="20" t="s">
         <v>246</v>
       </c>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29" t="s">
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28" t="s">
         <v>248</v>
       </c>
       <c r="F10" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="G10" s="29"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="29"/>
-      <c r="J10" s="29"/>
-      <c r="K10" s="29"/>
-      <c r="L10" s="29"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="28"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
@@ -1951,56 +1951,56 @@
       <c r="L11" s="8"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="29" t="s">
         <v>97</v>
       </c>
       <c r="B12" s="20" t="s">
         <v>246</v>
       </c>
-      <c r="C12" s="29" t="s">
+      <c r="C12" s="28" t="s">
         <v>144</v>
       </c>
-      <c r="D12" s="29" t="s">
+      <c r="D12" s="28" t="s">
         <v>199</v>
       </c>
-      <c r="E12" s="29" t="s">
+      <c r="E12" s="28" t="s">
         <v>248</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="G12" s="29" t="s">
+      <c r="G12" s="28" t="s">
         <v>310</v>
       </c>
-      <c r="H12" s="29" t="s">
+      <c r="H12" s="28" t="s">
         <v>251</v>
       </c>
-      <c r="I12" s="29" t="s">
+      <c r="I12" s="28" t="s">
         <v>305</v>
       </c>
-      <c r="J12" s="29" t="s">
+      <c r="J12" s="28" t="s">
         <v>319</v>
       </c>
-      <c r="K12" s="29"/>
-      <c r="L12" s="29"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="28"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="28"/>
+      <c r="A13" s="29"/>
       <c r="B13" s="20" t="s">
         <v>246</v>
       </c>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
       <c r="F13" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="G13" s="29"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="29"/>
-      <c r="J13" s="29"/>
-      <c r="K13" s="29"/>
-      <c r="L13" s="29"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="28"/>
     </row>
     <row r="14" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
@@ -2037,121 +2037,121 @@
       <c r="L14" s="8"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="28" t="s">
+      <c r="A15" s="29" t="s">
         <v>104</v>
       </c>
       <c r="B15" s="20" t="s">
         <v>246</v>
       </c>
-      <c r="C15" s="29" t="s">
+      <c r="C15" s="28" t="s">
         <v>145</v>
       </c>
-      <c r="D15" s="29" t="s">
+      <c r="D15" s="28" t="s">
         <v>201</v>
       </c>
-      <c r="E15" s="29" t="s">
+      <c r="E15" s="28" t="s">
         <v>248</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="G15" s="29" t="s">
+      <c r="G15" s="28" t="s">
         <v>310</v>
       </c>
-      <c r="H15" s="29" t="s">
+      <c r="H15" s="28" t="s">
         <v>226</v>
       </c>
-      <c r="I15" s="29" t="s">
+      <c r="I15" s="28" t="s">
         <v>305</v>
       </c>
-      <c r="J15" s="29" t="s">
+      <c r="J15" s="28" t="s">
         <v>319</v>
       </c>
-      <c r="K15" s="29"/>
-      <c r="L15" s="29"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="28"/>
+      <c r="A16" s="29"/>
       <c r="B16" s="20" t="s">
         <v>246</v>
       </c>
-      <c r="C16" s="29"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29" t="s">
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28" t="s">
         <v>248</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
-      <c r="K16" s="29"/>
-      <c r="L16" s="29"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="28"/>
+      <c r="K16" s="28"/>
+      <c r="L16" s="28"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A17" s="28" t="s">
+      <c r="A17" s="29" t="s">
         <v>108</v>
       </c>
       <c r="B17" s="20" t="s">
         <v>246</v>
       </c>
-      <c r="C17" s="29" t="s">
+      <c r="C17" s="28" t="s">
         <v>146</v>
       </c>
-      <c r="D17" s="29" t="s">
+      <c r="D17" s="28" t="s">
         <v>202</v>
       </c>
-      <c r="E17" s="29" t="s">
+      <c r="E17" s="28" t="s">
         <v>248</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="G17" s="29" t="s">
+      <c r="G17" s="28" t="s">
         <v>314</v>
       </c>
-      <c r="H17" s="29" t="s">
+      <c r="H17" s="28" t="s">
         <v>227</v>
       </c>
-      <c r="I17" s="29" t="s">
+      <c r="I17" s="28" t="s">
         <v>305</v>
       </c>
-      <c r="J17" s="29" t="s">
+      <c r="J17" s="28" t="s">
         <v>319</v>
       </c>
-      <c r="K17" s="29"/>
-      <c r="L17" s="29"/>
+      <c r="K17" s="28"/>
+      <c r="L17" s="28"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A18" s="28"/>
+      <c r="A18" s="29"/>
       <c r="B18" s="20" t="s">
         <v>246</v>
       </c>
-      <c r="C18" s="29"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="29" t="s">
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28" t="s">
         <v>248</v>
       </c>
       <c r="F18" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="G18" s="29"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
-      <c r="K18" s="29"/>
-      <c r="L18" s="29"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="28"/>
+      <c r="K18" s="28"/>
+      <c r="L18" s="28"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A19" s="28" t="s">
+      <c r="A19" s="29" t="s">
         <v>113</v>
       </c>
       <c r="B19" s="20" t="s">
         <v>246</v>
       </c>
-      <c r="C19" s="29" t="s">
+      <c r="C19" s="28" t="s">
         <v>146</v>
       </c>
       <c r="D19" s="20" t="s">
@@ -2163,7 +2163,7 @@
       <c r="F19" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="G19" s="29" t="s">
+      <c r="G19" s="28" t="s">
         <v>315</v>
       </c>
       <c r="H19" s="20" t="s">
@@ -2179,11 +2179,11 @@
       <c r="L19" s="20"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="28"/>
+      <c r="A20" s="29"/>
       <c r="B20" s="20" t="s">
         <v>246</v>
       </c>
-      <c r="C20" s="29"/>
+      <c r="C20" s="28"/>
       <c r="D20" s="20"/>
       <c r="E20" s="20" t="s">
         <v>248</v>
@@ -2191,7 +2191,7 @@
       <c r="F20" s="8" t="s">
         <v>219</v>
       </c>
-      <c r="G20" s="29"/>
+      <c r="G20" s="28"/>
       <c r="H20" s="20"/>
       <c r="I20" s="20"/>
       <c r="J20" s="20"/>
@@ -2199,56 +2199,56 @@
       <c r="L20" s="20"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A21" s="28" t="s">
+      <c r="A21" s="29" t="s">
         <v>118</v>
       </c>
       <c r="B21" s="20" t="s">
         <v>246</v>
       </c>
-      <c r="C21" s="29" t="s">
+      <c r="C21" s="28" t="s">
         <v>147</v>
       </c>
-      <c r="D21" s="29" t="s">
+      <c r="D21" s="28" t="s">
         <v>204</v>
       </c>
-      <c r="E21" s="29" t="s">
+      <c r="E21" s="28" t="s">
         <v>248</v>
       </c>
       <c r="F21" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="G21" s="29" t="s">
+      <c r="G21" s="28" t="s">
         <v>310</v>
       </c>
-      <c r="H21" s="29" t="s">
+      <c r="H21" s="28" t="s">
         <v>253</v>
       </c>
-      <c r="I21" s="29" t="s">
+      <c r="I21" s="28" t="s">
         <v>305</v>
       </c>
-      <c r="J21" s="29" t="s">
+      <c r="J21" s="28" t="s">
         <v>319</v>
       </c>
-      <c r="K21" s="29"/>
-      <c r="L21" s="29"/>
+      <c r="K21" s="28"/>
+      <c r="L21" s="28"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A22" s="28"/>
+      <c r="A22" s="29"/>
       <c r="B22" s="20" t="s">
         <v>246</v>
       </c>
-      <c r="C22" s="29"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="29"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="28"/>
       <c r="F22" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="G22" s="29"/>
-      <c r="H22" s="29"/>
-      <c r="I22" s="29"/>
-      <c r="J22" s="29"/>
-      <c r="K22" s="29"/>
-      <c r="L22" s="29"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="28"/>
+      <c r="I22" s="28"/>
+      <c r="J22" s="28"/>
+      <c r="K22" s="28"/>
+      <c r="L22" s="28"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="18" t="s">
@@ -2269,7 +2269,7 @@
       <c r="F23" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="G23" s="29" t="s">
+      <c r="G23" s="28" t="s">
         <v>310</v>
       </c>
       <c r="H23" s="20" t="s">
@@ -2295,7 +2295,7 @@
       <c r="F24" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="G24" s="29"/>
+      <c r="G24" s="28"/>
       <c r="H24" s="20"/>
       <c r="I24" s="21"/>
       <c r="J24" s="21"/>
@@ -2315,7 +2315,7 @@
       <c r="F25" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="G25" s="29"/>
+      <c r="G25" s="28"/>
       <c r="H25" s="20"/>
       <c r="I25" s="21"/>
       <c r="J25" s="21"/>
@@ -2333,7 +2333,7 @@
       <c r="F26" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="G26" s="29"/>
+      <c r="G26" s="28"/>
       <c r="H26" s="20"/>
       <c r="I26" s="21"/>
       <c r="J26" s="21"/>
@@ -2353,7 +2353,7 @@
       <c r="F27" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="G27" s="29"/>
+      <c r="G27" s="28"/>
       <c r="H27" s="20"/>
       <c r="I27" s="21"/>
       <c r="J27" s="21"/>
@@ -2371,7 +2371,7 @@
       <c r="F28" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="G28" s="29"/>
+      <c r="G28" s="28"/>
       <c r="H28" s="20"/>
       <c r="I28" s="21"/>
       <c r="J28" s="21"/>
@@ -2728,7 +2728,7 @@
       <c r="C44" s="27" t="s">
         <v>176</v>
       </c>
-      <c r="D44" s="29" t="s">
+      <c r="D44" s="28" t="s">
         <v>177</v>
       </c>
       <c r="E44" s="22" t="s">
@@ -2737,7 +2737,7 @@
       <c r="F44" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="G44" s="29" t="s">
+      <c r="G44" s="28" t="s">
         <v>310</v>
       </c>
       <c r="H44" s="20" t="s">
@@ -2756,12 +2756,12 @@
       <c r="A45" s="26"/>
       <c r="B45" s="22"/>
       <c r="C45" s="27"/>
-      <c r="D45" s="29"/>
+      <c r="D45" s="28"/>
       <c r="E45" s="22"/>
       <c r="F45" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="G45" s="29"/>
+      <c r="G45" s="28"/>
       <c r="H45" s="20"/>
       <c r="I45" s="20"/>
       <c r="J45" s="20"/>
@@ -2772,12 +2772,12 @@
       <c r="A46" s="26"/>
       <c r="B46" s="22"/>
       <c r="C46" s="27"/>
-      <c r="D46" s="29"/>
+      <c r="D46" s="28"/>
       <c r="E46" s="22"/>
       <c r="F46" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="G46" s="29"/>
+      <c r="G46" s="28"/>
       <c r="H46" s="20"/>
       <c r="I46" s="20"/>
       <c r="J46" s="20"/>
@@ -2785,25 +2785,25 @@
       <c r="L46" s="20"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A47" s="28" t="s">
+      <c r="A47" s="29" t="s">
         <v>136</v>
       </c>
       <c r="B47" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="C47" s="29" t="s">
+      <c r="C47" s="28" t="s">
         <v>181</v>
       </c>
-      <c r="D47" s="29" t="s">
+      <c r="D47" s="28" t="s">
         <v>182</v>
       </c>
-      <c r="E47" s="29" t="s">
+      <c r="E47" s="28" t="s">
         <v>248</v>
       </c>
       <c r="F47" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="G47" s="29" t="s">
+      <c r="G47" s="28" t="s">
         <v>310</v>
       </c>
       <c r="H47" s="20" t="s">
@@ -2819,15 +2819,15 @@
       <c r="L47" s="20"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A48" s="28"/>
+      <c r="A48" s="29"/>
       <c r="B48" s="22"/>
-      <c r="C48" s="29"/>
-      <c r="D48" s="29"/>
-      <c r="E48" s="29"/>
+      <c r="C48" s="28"/>
+      <c r="D48" s="28"/>
+      <c r="E48" s="28"/>
       <c r="F48" s="8" t="s">
         <v>259</v>
       </c>
-      <c r="G48" s="29"/>
+      <c r="G48" s="28"/>
       <c r="H48" s="20"/>
       <c r="I48" s="20"/>
       <c r="J48" s="20"/>
@@ -2835,15 +2835,15 @@
       <c r="L48" s="20"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A49" s="28"/>
+      <c r="A49" s="29"/>
       <c r="B49" s="22"/>
-      <c r="C49" s="29"/>
-      <c r="D49" s="29"/>
-      <c r="E49" s="29"/>
+      <c r="C49" s="28"/>
+      <c r="D49" s="28"/>
+      <c r="E49" s="28"/>
       <c r="F49" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="G49" s="29"/>
+      <c r="G49" s="28"/>
       <c r="H49" s="20"/>
       <c r="I49" s="20"/>
       <c r="J49" s="20"/>
@@ -2851,15 +2851,15 @@
       <c r="L49" s="20"/>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A50" s="28"/>
+      <c r="A50" s="29"/>
       <c r="B50" s="22"/>
-      <c r="C50" s="29"/>
-      <c r="D50" s="29"/>
-      <c r="E50" s="29"/>
+      <c r="C50" s="28"/>
+      <c r="D50" s="28"/>
+      <c r="E50" s="28"/>
       <c r="F50" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="G50" s="29"/>
+      <c r="G50" s="28"/>
       <c r="H50" s="20"/>
       <c r="I50" s="20"/>
       <c r="J50" s="20"/>
@@ -2867,25 +2867,25 @@
       <c r="L50" s="20"/>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A51" s="28" t="s">
+      <c r="A51" s="29" t="s">
         <v>229</v>
       </c>
       <c r="B51" s="20" t="s">
         <v>246</v>
       </c>
-      <c r="C51" s="29" t="s">
+      <c r="C51" s="28" t="s">
         <v>183</v>
       </c>
-      <c r="D51" s="29" t="s">
+      <c r="D51" s="28" t="s">
         <v>184</v>
       </c>
-      <c r="E51" s="29" t="s">
+      <c r="E51" s="28" t="s">
         <v>248</v>
       </c>
       <c r="F51" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="G51" s="29" t="s">
+      <c r="G51" s="28" t="s">
         <v>310</v>
       </c>
       <c r="H51" s="20" t="s">
@@ -2901,15 +2901,15 @@
       <c r="L51" s="20"/>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A52" s="28"/>
+      <c r="A52" s="29"/>
       <c r="B52" s="20"/>
-      <c r="C52" s="29"/>
-      <c r="D52" s="29"/>
-      <c r="E52" s="29"/>
+      <c r="C52" s="28"/>
+      <c r="D52" s="28"/>
+      <c r="E52" s="28"/>
       <c r="F52" s="8" t="s">
         <v>258</v>
       </c>
-      <c r="G52" s="29"/>
+      <c r="G52" s="28"/>
       <c r="H52" s="20"/>
       <c r="I52" s="20"/>
       <c r="J52" s="20"/>
@@ -2917,15 +2917,15 @@
       <c r="L52" s="20"/>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A53" s="28"/>
+      <c r="A53" s="29"/>
       <c r="B53" s="20"/>
-      <c r="C53" s="29"/>
-      <c r="D53" s="29"/>
-      <c r="E53" s="29"/>
+      <c r="C53" s="28"/>
+      <c r="D53" s="28"/>
+      <c r="E53" s="28"/>
       <c r="F53" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="G53" s="29"/>
+      <c r="G53" s="28"/>
       <c r="H53" s="20"/>
       <c r="I53" s="20"/>
       <c r="J53" s="20"/>
@@ -2933,15 +2933,15 @@
       <c r="L53" s="20"/>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A54" s="28"/>
+      <c r="A54" s="29"/>
       <c r="B54" s="20"/>
-      <c r="C54" s="29"/>
-      <c r="D54" s="29"/>
-      <c r="E54" s="29"/>
+      <c r="C54" s="28"/>
+      <c r="D54" s="28"/>
+      <c r="E54" s="28"/>
       <c r="F54" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="G54" s="29"/>
+      <c r="G54" s="28"/>
       <c r="H54" s="20"/>
       <c r="I54" s="20"/>
       <c r="J54" s="20"/>
@@ -2949,25 +2949,25 @@
       <c r="L54" s="20"/>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A55" s="28" t="s">
+      <c r="A55" s="29" t="s">
         <v>230</v>
       </c>
       <c r="B55" s="20" t="s">
         <v>246</v>
       </c>
-      <c r="C55" s="29" t="s">
+      <c r="C55" s="28" t="s">
         <v>186</v>
       </c>
-      <c r="D55" s="29" t="s">
+      <c r="D55" s="28" t="s">
         <v>187</v>
       </c>
-      <c r="E55" s="29" t="s">
+      <c r="E55" s="28" t="s">
         <v>248</v>
       </c>
       <c r="F55" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="G55" s="29" t="s">
+      <c r="G55" s="28" t="s">
         <v>310</v>
       </c>
       <c r="H55" s="20" t="s">
@@ -2983,15 +2983,15 @@
       <c r="L55" s="20"/>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A56" s="28"/>
+      <c r="A56" s="29"/>
       <c r="B56" s="20"/>
-      <c r="C56" s="29"/>
-      <c r="D56" s="29"/>
-      <c r="E56" s="29"/>
+      <c r="C56" s="28"/>
+      <c r="D56" s="28"/>
+      <c r="E56" s="28"/>
       <c r="F56" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="G56" s="29"/>
+      <c r="G56" s="28"/>
       <c r="H56" s="20"/>
       <c r="I56" s="20"/>
       <c r="J56" s="20"/>
@@ -2999,15 +2999,15 @@
       <c r="L56" s="20"/>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A57" s="28"/>
+      <c r="A57" s="29"/>
       <c r="B57" s="20"/>
-      <c r="C57" s="29"/>
-      <c r="D57" s="29"/>
-      <c r="E57" s="29"/>
+      <c r="C57" s="28"/>
+      <c r="D57" s="28"/>
+      <c r="E57" s="28"/>
       <c r="F57" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="G57" s="29"/>
+      <c r="G57" s="28"/>
       <c r="H57" s="20"/>
       <c r="I57" s="20"/>
       <c r="J57" s="20"/>
@@ -3637,7 +3637,7 @@
       <c r="F85" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="G85" s="29" t="s">
+      <c r="G85" s="28" t="s">
         <v>310</v>
       </c>
       <c r="H85" s="20" t="s">
@@ -3747,7 +3747,7 @@
       <c r="F90" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="G90" s="29" t="s">
+      <c r="G90" s="28" t="s">
         <v>318</v>
       </c>
       <c r="H90" s="20" t="s">
@@ -3773,7 +3773,7 @@
       <c r="F91" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="G91" s="29"/>
+      <c r="G91" s="28"/>
       <c r="H91" s="20"/>
       <c r="I91" s="21"/>
       <c r="J91" s="21"/>
@@ -3793,7 +3793,7 @@
       <c r="F92" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="G92" s="29"/>
+      <c r="G92" s="28"/>
       <c r="H92" s="20"/>
       <c r="I92" s="21"/>
       <c r="J92" s="21"/>
@@ -3811,7 +3811,7 @@
       <c r="F93" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="G93" s="29"/>
+      <c r="G93" s="28"/>
       <c r="H93" s="20"/>
       <c r="I93" s="21"/>
       <c r="J93" s="21"/>
@@ -3953,14 +3953,14 @@
       <c r="H99" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="I99" s="29" t="s">
+      <c r="I99" s="28" t="s">
         <v>305</v>
       </c>
-      <c r="J99" s="29" t="s">
+      <c r="J99" s="28" t="s">
         <v>319</v>
       </c>
-      <c r="K99" s="28"/>
-      <c r="L99" s="28"/>
+      <c r="K99" s="29"/>
+      <c r="L99" s="29"/>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A100" s="18"/>
@@ -3975,10 +3975,10 @@
       </c>
       <c r="G100" s="19"/>
       <c r="H100" s="21"/>
-      <c r="I100" s="29"/>
-      <c r="J100" s="29"/>
-      <c r="K100" s="28"/>
-      <c r="L100" s="28"/>
+      <c r="I100" s="28"/>
+      <c r="J100" s="28"/>
+      <c r="K100" s="29"/>
+      <c r="L100" s="29"/>
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A101" s="18"/>
@@ -3995,10 +3995,10 @@
       </c>
       <c r="G101" s="19"/>
       <c r="H101" s="21"/>
-      <c r="I101" s="29"/>
-      <c r="J101" s="29"/>
-      <c r="K101" s="28"/>
-      <c r="L101" s="28"/>
+      <c r="I101" s="28"/>
+      <c r="J101" s="28"/>
+      <c r="K101" s="29"/>
+      <c r="L101" s="29"/>
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A102" s="18"/>
@@ -4013,10 +4013,10 @@
       </c>
       <c r="G102" s="19"/>
       <c r="H102" s="21"/>
-      <c r="I102" s="29"/>
-      <c r="J102" s="29"/>
-      <c r="K102" s="28"/>
-      <c r="L102" s="28"/>
+      <c r="I102" s="28"/>
+      <c r="J102" s="28"/>
+      <c r="K102" s="29"/>
+      <c r="L102" s="29"/>
     </row>
     <row r="129" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H129" s="14"/>
@@ -4110,6 +4110,9 @@
     <mergeCell ref="E80:E84"/>
     <mergeCell ref="E85:E89"/>
     <mergeCell ref="E66:E69"/>
+    <mergeCell ref="D80:D84"/>
+    <mergeCell ref="D85:D89"/>
+    <mergeCell ref="D90:D93"/>
     <mergeCell ref="H17:H18"/>
     <mergeCell ref="H19:H20"/>
     <mergeCell ref="B58:B61"/>
@@ -4188,9 +4191,6 @@
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="B15:B16"/>
-    <mergeCell ref="D80:D84"/>
-    <mergeCell ref="D85:D89"/>
-    <mergeCell ref="D90:D93"/>
     <mergeCell ref="D58:D61"/>
     <mergeCell ref="D62:D65"/>
     <mergeCell ref="D66:D69"/>

</xml_diff>